<commit_message>
théo des nombres premiers up
</commit_message>
<xml_diff>
--- a/Mesures/Mesures.xlsx
+++ b/Mesures/Mesures.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14540" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14540" tabRatio="500" firstSheet="7" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Attaque Brutale" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="RSA Génération" sheetId="13" r:id="rId13"/>
     <sheet name="Chiffrement RSA" sheetId="14" r:id="rId14"/>
     <sheet name="Chiffrement ElG DES" sheetId="15" r:id="rId15"/>
+    <sheet name="Th des nombres premiers" sheetId="16" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="Attaque_brutale_moy10" localSheetId="0">'Attaque Brutale'!$A$1:$D$6</definedName>
@@ -44,6 +45,7 @@
     <definedName name="MillerRabin_proba_300_chiffres_moy_100" localSheetId="10">'Miller Rabin proba'!$A$1:$D$256</definedName>
     <definedName name="RSA_generation" localSheetId="12">'RSA Génération'!$A$1:$B$45</definedName>
     <definedName name="test_puissmod__moy_100" localSheetId="11">'test puiss mod'!$A$1:$C$169</definedName>
+    <definedName name="Théorème_des_nombres_premiers" localSheetId="15">'Th des nombres premiers'!$A$1:$B$59</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -112,7 +114,7 @@
     </textPr>
   </connection>
   <connection id="7" name="-Chiffrement ElGamal_DES" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/Ludo/Documents/GitHub/tipe/Mesures/-Chiffrement ElGamal_DES.txt" thousands=" " tab="0" semicolon="1">
+    <textPr fileType="mac" sourceFile="/Users/Ludo/Documents/GitHub/tipe/Mesures/-Chiffrement ElGamal_DES.txt" thousands=" " tab="0" semicolon="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -198,6 +200,14 @@
     <textPr fileType="mac" sourceFile="/Users/Ludo/Documents/GitHub/tipe/Mesures/-test-puissmod (moy 100).txt" thousands=" " semicolon="1">
       <textFields count="3">
         <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="16" name="-Théorème des nombres premiers" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/Ludo/Documents/GitHub/tipe/Mesures/-Théorème des nombres premiers.txt" thousands=" " semicolon="1">
+      <textFields count="2">
         <textField/>
         <textField/>
       </textFields>
@@ -3459,11 +3469,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1696399200"/>
-        <c:axId val="-1696396880"/>
+        <c:axId val="828971056"/>
+        <c:axId val="828973744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1696399200"/>
+        <c:axId val="828971056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3520,12 +3530,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1696396880"/>
+        <c:crossAx val="828973744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1696396880"/>
+        <c:axId val="828973744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3582,7 +3592,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1696399200"/>
+        <c:crossAx val="828971056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5108,11 +5118,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1697373488"/>
-        <c:axId val="-1697371008"/>
+        <c:axId val="935488704"/>
+        <c:axId val="935490752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1697373488"/>
+        <c:axId val="935488704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5169,12 +5179,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1697371008"/>
+        <c:crossAx val="935490752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1697371008"/>
+        <c:axId val="935490752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5231,7 +5241,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1697373488"/>
+        <c:crossAx val="935488704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6555,11 +6565,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1697326304"/>
-        <c:axId val="-1788633904"/>
+        <c:axId val="870903248"/>
+        <c:axId val="870905728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1697326304"/>
+        <c:axId val="870903248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6616,12 +6626,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1788633904"/>
+        <c:crossAx val="870905728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1788633904"/>
+        <c:axId val="870905728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6678,7 +6688,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1697326304"/>
+        <c:crossAx val="870903248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8415,11 +8425,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1697322160"/>
-        <c:axId val="-1697320096"/>
+        <c:axId val="935514096"/>
+        <c:axId val="935516576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1697322160"/>
+        <c:axId val="935514096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8476,12 +8486,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1697320096"/>
+        <c:crossAx val="935516576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1697320096"/>
+        <c:axId val="935516576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8538,7 +8548,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1697322160"/>
+        <c:crossAx val="935514096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11701,11 +11711,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1697274992"/>
-        <c:axId val="-1697272512"/>
+        <c:axId val="935558576"/>
+        <c:axId val="935561056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1697274992"/>
+        <c:axId val="935558576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11762,12 +11772,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1697272512"/>
+        <c:crossAx val="935561056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1697272512"/>
+        <c:axId val="935561056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11824,7 +11834,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1697274992"/>
+        <c:crossAx val="935558576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14888,6 +14898,10 @@
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="-Chiffrement ElGamal_DES" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
+<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="-Théorème des nombres premiers" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="-Attaque_Calcul-indexe(modele)" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
@@ -30386,6 +30400,497 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>10</v>
+      </c>
+      <c r="B1">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>21.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>30</v>
+      </c>
+      <c r="B3">
+        <v>52.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>40</v>
+      </c>
+      <c r="B4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>65.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>60</v>
+      </c>
+      <c r="B6">
+        <v>66.099999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>70</v>
+      </c>
+      <c r="B7">
+        <v>65.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>80</v>
+      </c>
+      <c r="B8">
+        <v>106.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>90</v>
+      </c>
+      <c r="B9">
+        <v>148.30000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>100</v>
+      </c>
+      <c r="B10">
+        <v>79.400000000000006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>110</v>
+      </c>
+      <c r="B11">
+        <v>61.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>120</v>
+      </c>
+      <c r="B12">
+        <v>63.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>130</v>
+      </c>
+      <c r="B13">
+        <v>120.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>140</v>
+      </c>
+      <c r="B14">
+        <v>168.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>150</v>
+      </c>
+      <c r="B15">
+        <v>167.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>160</v>
+      </c>
+      <c r="B16">
+        <v>170.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>170</v>
+      </c>
+      <c r="B17">
+        <v>305.89999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>180</v>
+      </c>
+      <c r="B18">
+        <v>246.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>190</v>
+      </c>
+      <c r="B19">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>200</v>
+      </c>
+      <c r="B20">
+        <v>390.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>210</v>
+      </c>
+      <c r="B21">
+        <v>161.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>220</v>
+      </c>
+      <c r="B22">
+        <v>314.89999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>230</v>
+      </c>
+      <c r="B23">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>240</v>
+      </c>
+      <c r="B24">
+        <v>362.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>250</v>
+      </c>
+      <c r="B25">
+        <v>182.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>260</v>
+      </c>
+      <c r="B26">
+        <v>283.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>270</v>
+      </c>
+      <c r="B27">
+        <v>222.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>280</v>
+      </c>
+      <c r="B28">
+        <v>488.7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>290</v>
+      </c>
+      <c r="B29">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>300</v>
+      </c>
+      <c r="B30">
+        <v>761.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>310</v>
+      </c>
+      <c r="B31">
+        <v>346.8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>320</v>
+      </c>
+      <c r="B32">
+        <v>570.79999999999995</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>330</v>
+      </c>
+      <c r="B33">
+        <v>328.1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>340</v>
+      </c>
+      <c r="B34">
+        <v>309.7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>350</v>
+      </c>
+      <c r="B35">
+        <v>260.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>360</v>
+      </c>
+      <c r="B36">
+        <v>222.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>370</v>
+      </c>
+      <c r="B37">
+        <v>326.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>380</v>
+      </c>
+      <c r="B38">
+        <v>396.4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>390</v>
+      </c>
+      <c r="B39">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>400</v>
+      </c>
+      <c r="B40">
+        <v>297.10000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>410</v>
+      </c>
+      <c r="B41">
+        <v>258.2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>420</v>
+      </c>
+      <c r="B42">
+        <v>261.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>430</v>
+      </c>
+      <c r="B43">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>440</v>
+      </c>
+      <c r="B44">
+        <v>432.1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>450</v>
+      </c>
+      <c r="B45">
+        <v>447.2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>460</v>
+      </c>
+      <c r="B46">
+        <v>529.79999999999995</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>470</v>
+      </c>
+      <c r="B47">
+        <v>628.20000000000005</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>480</v>
+      </c>
+      <c r="B48">
+        <v>398.2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>490</v>
+      </c>
+      <c r="B49">
+        <v>685.9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>500</v>
+      </c>
+      <c r="B50">
+        <v>561.6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>510</v>
+      </c>
+      <c r="B51">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>520</v>
+      </c>
+      <c r="B52">
+        <v>762.4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>530</v>
+      </c>
+      <c r="B53">
+        <v>367.7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>540</v>
+      </c>
+      <c r="B54">
+        <v>291.39999999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>550</v>
+      </c>
+      <c r="B55">
+        <v>825.1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>560</v>
+      </c>
+      <c r="B56">
+        <v>823.3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>570</v>
+      </c>
+      <c r="B57">
+        <v>484.6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>580</v>
+      </c>
+      <c r="B58">
+        <v>1059.7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>590</v>
+      </c>
+      <c r="B59">
+        <v>640.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B500"/>
@@ -45901,7 +46406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="L5" sqref="L4:L5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
MAJ RSA fonction de p et EG fonction de p
</commit_message>
<xml_diff>
--- a/Mesures/Mesures.xlsx
+++ b/Mesures/Mesures.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14540" tabRatio="500" firstSheet="8" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14540" tabRatio="500" firstSheet="9" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Attaque Brutale" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,10 @@
     <sheet name="Miller Rabin proba" sheetId="11" r:id="rId11"/>
     <sheet name="test puiss mod" sheetId="12" r:id="rId12"/>
     <sheet name="RSA Génération" sheetId="13" r:id="rId13"/>
-    <sheet name="Chiffrement RSA" sheetId="14" r:id="rId14"/>
-    <sheet name="Chiffrement ElG DES" sheetId="15" r:id="rId15"/>
+    <sheet name="Chiffrement RSA" sheetId="18" r:id="rId14"/>
+    <sheet name="Chiffrement EG DES" sheetId="15" r:id="rId15"/>
     <sheet name="Th des nombres premiers" sheetId="16" r:id="rId16"/>
-    <sheet name="El Gamal fonction de p" sheetId="17" r:id="rId17"/>
+    <sheet name="EG fonction de p" sheetId="19" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="Attaque_brutale_moy10" localSheetId="0">'Attaque Brutale'!$A$1:$D$6</definedName>
@@ -37,10 +37,10 @@
     <definedName name="Attaque_rho_pollard" localSheetId="3">'Attaque rho'!$A$2:$B$12</definedName>
     <definedName name="Attaque_Shanks_modele" localSheetId="4">'Attaque shanks mod'!$A$2:$B$99</definedName>
     <definedName name="Attaque_Shanks_moy100" localSheetId="5">'Attaque shanks moy 100'!$A$2:$D$8</definedName>
-    <definedName name="Chiffrement_ElGamal_DES" localSheetId="14">'Chiffrement ElG DES'!$A$1:$E$220</definedName>
-    <definedName name="Chiffrement_ElGamal_fonction_de_p" localSheetId="16">'El Gamal fonction de p'!$A$1:$E$58</definedName>
+    <definedName name="Chiffrement_ElGamal_DES" localSheetId="14">'Chiffrement EG DES'!$A$1:$E$220</definedName>
+    <definedName name="Chiffrement_ElGamal_fonction_de_p" localSheetId="16">'EG fonction de p'!$A$2:$E$59</definedName>
     <definedName name="Chiffrement_ElGamal_n_200" localSheetId="6">'Chiffrement El gamal'!$A$1:$E$331</definedName>
-    <definedName name="Chiffrement_RSA" localSheetId="13">'Chiffrement RSA'!$A$2:$E$85</definedName>
+    <definedName name="Chiffrement_RSA" localSheetId="13">'Chiffrement RSA'!$A$2:$E$165</definedName>
     <definedName name="Générateur_moy_100" localSheetId="7">'Générateur k illimité'!$A$1:$G$71</definedName>
     <definedName name="Génerateur_moy10_k_500" localSheetId="8">'Générateur 500'!$A$2:$D$58</definedName>
     <definedName name="MillerRabin_génération_moy_100" localSheetId="9">'Miller Rabin gen'!$A$1:$D$262</definedName>
@@ -115,7 +115,18 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="7" name="-Chiffrement ElGamal_DES" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="7" name="-Chiffrement ElGamal fonction de p" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/Ludo/Documents/GitHub/tipe/Mesures/-Chiffrement ElGamal fonction de p.txt" thousands=" " tab="0" semicolon="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="8" name="-Chiffrement ElGamal_DES" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/Ludo/Documents/GitHub/tipe/Mesures/-Chiffrement ElGamal_DES.txt" thousands=" " tab="0" semicolon="1">
       <textFields count="5">
         <textField/>
@@ -126,7 +137,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="8" name="-Chiffrement_ElGamal(n=200)" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="9" name="-Chiffrement_ElGamal(n=200)" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/Ludo/Documents/GitHub/tipe/Mesures/-Chiffrement_ElGamal(n=200).txt" thousands=" " semicolon="1">
       <textFields count="5">
         <textField/>
@@ -137,8 +148,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="9" name="-Chiffrement_RSA" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="850" sourceFile="E:\Users\Ludo\Documents\GitHub\TIPE-2018\Mesures\-Chiffrement_RSA.txt" thousands=" " tab="0" semicolon="1">
+  <connection id="10" name="-Chiffrement_RSA" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/Ludo/Documents/GitHub/tipe/Mesures/-Chiffrement_RSA.txt" thousands=" " semicolon="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -148,7 +159,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="10" name="-Générateur(moy 100)" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="11" name="-Générateur(moy 100)" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/Ludo/Documents/GitHub/tipe/Mesures/-Générateur(moy 100).txt" thousands=" " semicolon="1">
       <textFields count="7">
         <textField/>
@@ -161,7 +172,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="11" name="-Génerateur(moy10,k=500)" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="12" name="-Génerateur(moy10,k=500)" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/Ludo/Documents/GitHub/tipe/Mesures/-Génerateur(moy10,k=500).txt" thousands=" " semicolon="1">
       <textFields count="4">
         <textField/>
@@ -171,7 +182,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="12" name="-MillerRabin_génération(moy 100)" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="13" name="-MillerRabin_génération(moy 100)" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/Ludo/Documents/GitHub/tipe/Mesures/-MillerRabin_génération(moy 100).txt" thousands=" " semicolon="1">
       <textFields count="4">
         <textField/>
@@ -181,7 +192,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="13" name="-MillerRabin_proba(300 chiffres,moy 100)" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="14" name="-MillerRabin_proba(300 chiffres,moy 100)" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/Ludo/Documents/GitHub/tipe/Mesures/-MillerRabin_proba(300 chiffres,moy 100).txt" thousands=" " semicolon="1">
       <textFields count="3">
         <textField/>
@@ -190,7 +201,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="14" name="-RSA_generation" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="15" name="-RSA_generation" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="850" sourceFile="E:\Users\Ludo\Documents\GitHub\TIPE-2018\Mesures\-RSA_generation.txt" thousands=" " tab="0" semicolon="1">
       <textFields count="2">
         <textField/>
@@ -198,7 +209,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="15" name="-test-puissmod (moy 100)" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="16" name="-test-puissmod (moy 100)" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/Ludo/Documents/GitHub/tipe/Mesures/-test-puissmod (moy 100).txt" thousands=" " semicolon="1">
       <textFields count="3">
         <textField/>
@@ -207,20 +218,9 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="16" name="-Théorème des nombres premiers" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="17" name="-Théorème des nombres premiers" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/Ludo/Documents/GitHub/tipe/Mesures/-Théorème des nombres premiers.txt" thousands=" " semicolon="1">
       <textFields count="2">
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="17" name="Chiffrement ElGamal fonction de p" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/Ludo/Documents/GitHub/tipe/Mesures/Chiffrement ElGamal fonction de p.txt" thousands=" " semicolon="1">
-      <textFields count="5">
-        <textField/>
-        <textField/>
-        <textField/>
         <textField/>
         <textField/>
       </textFields>
@@ -230,7 +230,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="22">
   <si>
     <t>n</t>
   </si>
@@ -3482,11 +3482,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1119832464"/>
-        <c:axId val="-1119830256"/>
+        <c:axId val="1617736128"/>
+        <c:axId val="1617838608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1119832464"/>
+        <c:axId val="1617736128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3543,12 +3543,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1119830256"/>
+        <c:crossAx val="1617838608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1119830256"/>
+        <c:axId val="1617838608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3605,7 +3605,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1119832464"/>
+        <c:crossAx val="1617736128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5131,11 +5131,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1224946368"/>
-        <c:axId val="-1224943888"/>
+        <c:axId val="1616486400"/>
+        <c:axId val="1616488448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1224946368"/>
+        <c:axId val="1616486400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5192,12 +5192,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1224943888"/>
+        <c:crossAx val="1616488448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1224943888"/>
+        <c:axId val="1616488448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5254,7 +5254,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1224946368"/>
+        <c:crossAx val="1616486400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6577,11 +6577,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1224925680"/>
-        <c:axId val="-1224923200"/>
+        <c:axId val="1713056848"/>
+        <c:axId val="1713058640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1224925680"/>
+        <c:axId val="1713056848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6638,12 +6638,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1224923200"/>
+        <c:crossAx val="1713058640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1224923200"/>
+        <c:axId val="1713058640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6700,7 +6700,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1224925680"/>
+        <c:crossAx val="1713056848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8437,11 +8437,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1119776992"/>
-        <c:axId val="-1119774512"/>
+        <c:axId val="1618654416"/>
+        <c:axId val="1618656896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1119776992"/>
+        <c:axId val="1618654416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8498,12 +8498,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1119774512"/>
+        <c:crossAx val="1618656896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1119774512"/>
+        <c:axId val="1618656896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8560,7 +8560,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1119776992"/>
+        <c:crossAx val="1618654416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11722,11 +11722,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1227028864"/>
-        <c:axId val="-1227026800"/>
+        <c:axId val="1713105152"/>
+        <c:axId val="1713107632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1227028864"/>
+        <c:axId val="1713105152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11783,12 +11783,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1227026800"/>
+        <c:crossAx val="1713107632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1227026800"/>
+        <c:axId val="1713107632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11845,7 +11845,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1227028864"/>
+        <c:crossAx val="1713105152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14885,35 +14885,35 @@
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="-MillerRabin_génération(moy 100)" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="-MillerRabin_génération(moy 100)" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="-MillerRabin_proba(300 chiffres,moy 100)" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="-MillerRabin_proba(300 chiffres,moy 100)" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="-test-puissmod (moy 100)" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="-test-puissmod (moy 100)" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="-RSA_generation" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="-RSA_generation" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="-Chiffrement_RSA" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="-Chiffrement_RSA" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="-Chiffrement ElGamal_DES" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="-Chiffrement ElGamal_DES" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="-Théorème des nombres premiers" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="-Théorème des nombres premiers" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Chiffrement ElGamal fonction de p" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="-Chiffrement ElGamal fonction de p" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14937,15 +14937,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="-Chiffrement_ElGamal(n=200)" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="-Chiffrement_ElGamal(n=200)" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="-Générateur(moy 100)" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="-Générateur(moy 100)" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="-Génerateur(moy10,k=500)" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="-Génerateur(moy10,k=500)" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -23115,7 +23115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
@@ -23492,17 +23492,17 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -23510,16 +23510,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -24360,593 +24360,1953 @@
         <v>500</v>
       </c>
       <c r="B51">
-        <v>0.92448951859878403</v>
+        <v>0.91943478949833601</v>
       </c>
       <c r="C51">
-        <v>0.92339157759997703</v>
+        <v>0.91886202940222494</v>
       </c>
       <c r="D51" s="2">
-        <v>0.92417934380209699</v>
+        <v>0.91919492190354501</v>
       </c>
       <c r="E51" s="2">
-        <v>0.92537020580020901</v>
+        <v>0.92057224879972599</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>583</v>
+        <v>510</v>
       </c>
       <c r="B52">
-        <v>0.92388212170080797</v>
+        <v>0.919335772996419</v>
       </c>
       <c r="C52">
-        <v>0.92291087210032796</v>
+        <v>0.91871103409939603</v>
       </c>
       <c r="D52" s="2">
-        <v>0.92280852359908705</v>
+        <v>0.91888973509776395</v>
       </c>
       <c r="E52" s="2">
-        <v>0.924936281001282</v>
+        <v>0.920641464802611</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>666</v>
+        <v>520</v>
       </c>
       <c r="B53">
-        <v>1.1548776437000901</v>
+        <v>0.92057598310493605</v>
       </c>
       <c r="C53">
-        <v>1.15440878770059</v>
+        <v>0.91989863979833897</v>
       </c>
       <c r="D53" s="2">
-        <v>1.1539686236981599</v>
+        <v>0.92016490380774396</v>
       </c>
       <c r="E53" s="2">
-        <v>1.1560992088987401</v>
+        <v>0.922372780602017</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>749</v>
+        <v>530</v>
       </c>
       <c r="B54">
-        <v>1.15439145910022</v>
+        <v>0.92045788050163502</v>
       </c>
       <c r="C54">
-        <v>1.1534300020019099</v>
+        <v>0.91944075930077795</v>
       </c>
       <c r="D54" s="2">
-        <v>1.1537003545003199</v>
+        <v>0.91950540470570497</v>
       </c>
       <c r="E54" s="2">
-        <v>1.15563560200062</v>
+        <v>0.92167570930760101</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>832</v>
+        <v>540</v>
       </c>
       <c r="B55">
-        <v>1.38564199650027</v>
+        <v>0.91935469710151596</v>
       </c>
       <c r="C55">
-        <v>1.3855663201989901</v>
+        <v>0.91874480650585599</v>
       </c>
       <c r="D55" s="2">
-        <v>1.3852099439995</v>
+        <v>0.91870069739525195</v>
       </c>
       <c r="E55" s="2">
-        <v>1.3885459638004201</v>
+        <v>0.92065362319845001</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>915</v>
+        <v>550</v>
       </c>
       <c r="B56">
-        <v>1.38689154030071</v>
+        <v>0.92005975200008805</v>
       </c>
       <c r="C56">
-        <v>1.38488221379957</v>
+        <v>0.91948698619380598</v>
       </c>
       <c r="D56" s="2">
-        <v>1.3849650686988699</v>
+        <v>0.91903721970011198</v>
       </c>
       <c r="E56" s="2">
-        <v>1.3879301041990399</v>
+        <v>0.92103212439833404</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>998</v>
+        <v>560</v>
       </c>
       <c r="B57">
-        <v>1.61716500869915</v>
+        <v>0.92033386200346201</v>
       </c>
       <c r="C57">
-        <v>1.61594315349721</v>
+        <v>0.91954363989789201</v>
       </c>
       <c r="D57" s="2">
-        <v>1.6158993193985201</v>
+        <v>0.91959817030146895</v>
       </c>
       <c r="E57" s="2">
-        <v>1.6199871638022101</v>
+        <v>0.92305132869951101</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>1081</v>
+        <v>570</v>
       </c>
       <c r="B58">
-        <v>1.6170410633985699</v>
+        <v>0.92026614050264399</v>
       </c>
       <c r="C58">
-        <v>1.6153697958998201</v>
+        <v>0.91950660019792796</v>
       </c>
       <c r="D58" s="2">
-        <v>1.6155303217994501</v>
+        <v>0.91943206470314098</v>
       </c>
       <c r="E58" s="2">
-        <v>1.61871744680174</v>
+        <v>0.92167280559951903</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>1164</v>
+        <v>580</v>
       </c>
       <c r="B59">
-        <v>1.84923571320068</v>
+        <v>0.92241561789996895</v>
       </c>
       <c r="C59">
-        <v>1.84642793020138</v>
+        <v>0.92141880340204796</v>
       </c>
       <c r="D59" s="2">
-        <v>1.8461463945994101</v>
+        <v>0.92175823819416103</v>
       </c>
       <c r="E59" s="2">
-        <v>1.8506708872016999</v>
+        <v>0.92389325629774199</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>1247</v>
+        <v>590</v>
       </c>
       <c r="B60">
-        <v>1.85077662210132</v>
+        <v>0.92420580590260204</v>
       </c>
       <c r="C60">
-        <v>1.8471348775005001</v>
+        <v>0.92297516049584305</v>
       </c>
       <c r="D60" s="2">
-        <v>1.84770604229925</v>
+        <v>0.923638451704755</v>
       </c>
       <c r="E60" s="2">
-        <v>1.85212962750265</v>
+        <v>0.92630721579771402</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>1330</v>
+        <v>600</v>
       </c>
       <c r="B61">
-        <v>2.0792909563984701</v>
+        <v>0.91969638000155096</v>
       </c>
       <c r="C61">
-        <v>2.0770796074018998</v>
+        <v>0.919532704103039</v>
       </c>
       <c r="D61" s="2">
-        <v>2.0769231768997898</v>
+        <v>0.91931368050281803</v>
       </c>
       <c r="E61" s="2">
-        <v>2.0814406898996798</v>
+        <v>0.92131407010019695</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>1413</v>
+        <v>610</v>
       </c>
       <c r="B62">
-        <v>2.08082759159988</v>
+        <v>0.91981994509696896</v>
       </c>
       <c r="C62">
-        <v>2.07704272090159</v>
+        <v>0.91921127859677598</v>
       </c>
       <c r="D62" s="2">
-        <v>2.0772477312006199</v>
+        <v>0.919130758101528</v>
       </c>
       <c r="E62" s="2">
-        <v>2.0826132616992199</v>
+        <v>0.92116900160181103</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>1496</v>
+        <v>620</v>
       </c>
       <c r="B63">
-        <v>2.3111542399994498</v>
+        <v>0.91987791619758297</v>
       </c>
       <c r="C63">
-        <v>2.3087513166989</v>
+        <v>0.91906065810326198</v>
       </c>
       <c r="D63" s="2">
-        <v>2.3078786508980502</v>
+        <v>0.919430920196464</v>
       </c>
       <c r="E63" s="2">
-        <v>2.3142482793002199</v>
+        <v>0.92122319210320702</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>1579</v>
+        <v>630</v>
       </c>
       <c r="B64">
-        <v>2.3117302255002801</v>
+        <v>0.91997354820050503</v>
       </c>
       <c r="C64">
-        <v>2.30820002760119</v>
+        <v>0.91899232789582996</v>
       </c>
       <c r="D64" s="2">
-        <v>2.3088033395000802</v>
+        <v>0.91910050920123398</v>
       </c>
       <c r="E64" s="2">
-        <v>2.3128195776003801</v>
+        <v>0.92105946690135099</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>1662</v>
+        <v>640</v>
       </c>
       <c r="B65">
-        <v>2.54227149650105</v>
+        <v>0.91966209530364695</v>
       </c>
       <c r="C65">
-        <v>2.5392136873990201</v>
+        <v>0.91871763920498695</v>
       </c>
       <c r="D65" s="2">
-        <v>2.5397528821984401</v>
+        <v>0.91902283470553803</v>
       </c>
       <c r="E65" s="2">
-        <v>2.5442274139004399</v>
+        <v>0.92052959850407201</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>1745</v>
+        <v>650</v>
       </c>
       <c r="B66">
-        <v>2.5428949605011399</v>
+        <v>0.920070676006435</v>
       </c>
       <c r="C66">
-        <v>2.53902974829579</v>
+        <v>0.919179392700607</v>
       </c>
       <c r="D66" s="2">
-        <v>2.5400896978004299</v>
+        <v>0.91887423370353605</v>
       </c>
       <c r="E66" s="2">
-        <v>2.5443249798015999</v>
+        <v>0.92088995039666699</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>1828</v>
+        <v>660</v>
       </c>
       <c r="B67">
-        <v>2.7741687695033699</v>
+        <v>0.91996043940307504</v>
       </c>
       <c r="C67">
-        <v>2.7699574161993898</v>
+        <v>0.91895356179884402</v>
       </c>
       <c r="D67" s="2">
-        <v>2.7708509844003801</v>
+        <v>0.91897869210078997</v>
       </c>
       <c r="E67" s="2">
-        <v>2.7758213149019801</v>
+        <v>0.92102844069304401</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>1911</v>
+        <v>670</v>
       </c>
       <c r="B68">
-        <v>2.77523935579993</v>
+        <v>1.1494392419976001</v>
       </c>
       <c r="C68">
-        <v>2.7703980756989002</v>
+        <v>1.1485142970064699</v>
       </c>
       <c r="D68" s="2">
-        <v>2.77003198079837</v>
+        <v>1.14873855480109</v>
       </c>
       <c r="E68" s="2">
-        <v>2.77650629879972</v>
+        <v>1.1508668865935701</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>1994</v>
+        <v>680</v>
       </c>
       <c r="B69">
-        <v>3.0064893082006101</v>
+        <v>1.14961439950566</v>
       </c>
       <c r="C69">
-        <v>3.0019949998019002</v>
+        <v>1.14883132230606</v>
       </c>
       <c r="D69" s="2">
-        <v>3.0010721826023601</v>
+        <v>1.1485960901016301</v>
       </c>
       <c r="E69" s="2">
-        <v>3.0074823880975599</v>
+        <v>1.15102542960084</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>2077</v>
+        <v>690</v>
       </c>
       <c r="B70">
-        <v>3.0047839199989501</v>
+        <v>1.14917643619846</v>
       </c>
       <c r="C70">
-        <v>3.0005700640020199</v>
+        <v>1.14828360020183</v>
       </c>
       <c r="D70" s="2">
-        <v>3.00135763599901</v>
+        <v>1.1483450528030501</v>
       </c>
       <c r="E70" s="2">
-        <v>3.0072964612987501</v>
+        <v>1.1505785810964799</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>2160</v>
+        <v>700</v>
       </c>
       <c r="B71">
-        <v>3.2354625024003298</v>
+        <v>1.1491033290963899</v>
       </c>
       <c r="C71">
-        <v>3.2312648426006398</v>
+        <v>1.1479954272101101</v>
       </c>
       <c r="D71" s="2">
-        <v>3.2317017569992399</v>
+        <v>1.14797085960308</v>
       </c>
       <c r="E71" s="2">
-        <v>3.23821297069916</v>
+        <v>1.15071746189642</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>2243</v>
+        <v>710</v>
       </c>
       <c r="B72">
-        <v>3.22337480519854</v>
+        <v>1.14901655010471</v>
       </c>
       <c r="C72">
-        <v>3.2188382781001499</v>
+        <v>1.1479696468988501</v>
       </c>
       <c r="D72" s="2">
-        <v>3.2185373202999399</v>
+        <v>1.14801028729416</v>
       </c>
       <c r="E72" s="2">
-        <v>3.2266523780042902</v>
+        <v>1.15047745379415</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>2326</v>
+        <v>720</v>
       </c>
       <c r="B73">
-        <v>3.4530660588028601</v>
+        <v>1.1500550935001199</v>
       </c>
       <c r="C73">
-        <v>3.4469978186021701</v>
+        <v>1.14937349510146</v>
       </c>
       <c r="D73" s="2">
-        <v>3.4468672844988699</v>
+        <v>1.14905126269004</v>
       </c>
       <c r="E73" s="2">
-        <v>3.4548454540021298</v>
+        <v>1.1517044752967101</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>2409</v>
+        <v>730</v>
       </c>
       <c r="B74">
-        <v>3.45246772610116</v>
+        <v>1.1497207466963999</v>
       </c>
       <c r="C74">
-        <v>3.4471679462021698</v>
+        <v>1.14859566270752</v>
       </c>
       <c r="D74" s="2">
-        <v>3.4486230679009102</v>
+        <v>1.14875254140351</v>
       </c>
       <c r="E74" s="2">
-        <v>3.4544709747977298</v>
+        <v>1.1507954462955201</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>2492</v>
+        <v>740</v>
       </c>
       <c r="B75">
-        <v>3.68389598089815</v>
+        <v>1.1499174323980601</v>
       </c>
       <c r="C75">
-        <v>3.6775013342004899</v>
+        <v>1.14880606139195</v>
       </c>
       <c r="D75" s="2">
-        <v>3.6784485956992201</v>
+        <v>1.14846880350523</v>
       </c>
       <c r="E75" s="2">
-        <v>3.6863269559984402</v>
+        <v>1.1510198026982801</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>2575</v>
+        <v>750</v>
       </c>
       <c r="B76">
-        <v>3.6827995692001401</v>
+        <v>1.1496964483041601</v>
       </c>
       <c r="C76">
-        <v>3.6775139375986301</v>
+        <v>1.1484656001004601</v>
       </c>
       <c r="D76" s="2">
-        <v>3.6774336517009898</v>
+        <v>1.1482585594931101</v>
       </c>
       <c r="E76" s="2">
-        <v>3.68622713070144</v>
+        <v>1.1511502542052701</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>2658</v>
+        <v>760</v>
       </c>
       <c r="B77">
-        <v>3.9125397755018598</v>
+        <v>1.14976424390333</v>
       </c>
       <c r="C77">
-        <v>3.9069434099015701</v>
+        <v>1.1486965388030499</v>
       </c>
       <c r="D77" s="2">
-        <v>3.9071265521011802</v>
+        <v>1.1485277488027299</v>
       </c>
       <c r="E77" s="2">
-        <v>3.9152474940019601</v>
+        <v>1.1510674046949101</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>2741</v>
+        <v>770</v>
       </c>
       <c r="B78">
-        <v>3.9134088366976298</v>
+        <v>1.14982071530248</v>
       </c>
       <c r="C78">
-        <v>3.9071483164032501</v>
+        <v>1.14864648060902</v>
       </c>
       <c r="D78" s="2">
-        <v>3.9076248787019701</v>
+        <v>1.1487064590110001</v>
       </c>
       <c r="E78" s="2">
-        <v>3.9154213372996298</v>
+        <v>1.1511228030998599</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>2824</v>
+        <v>780</v>
       </c>
       <c r="B79">
-        <v>4.14514273610075</v>
+        <v>1.1501934658052</v>
       </c>
       <c r="C79">
-        <v>4.13869946940176</v>
+        <v>1.1488366692021299</v>
       </c>
       <c r="D79" s="2">
-        <v>4.1380854752973297</v>
+        <v>1.14894405909435</v>
       </c>
       <c r="E79" s="2">
-        <v>4.1484387924985597</v>
+        <v>1.1514115545927699</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>2907</v>
+        <v>790</v>
       </c>
       <c r="B80">
-        <v>4.16121216540341</v>
+        <v>1.1506431986024801</v>
       </c>
       <c r="C80">
-        <v>4.1553411544995402</v>
+        <v>1.1492435174965001</v>
       </c>
       <c r="D80" s="2">
-        <v>4.1548015606029303</v>
+        <v>1.14932523599709</v>
       </c>
       <c r="E80" s="2">
-        <v>4.1654067057992501</v>
+        <v>1.1517276222017201</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>2990</v>
+        <v>800</v>
       </c>
       <c r="B81">
-        <v>4.3926759652978902</v>
+        <v>1.1501885854056999</v>
       </c>
       <c r="C81">
-        <v>4.3864021097011499</v>
+        <v>1.1491218023002101</v>
       </c>
       <c r="D81" s="2">
-        <v>4.3859517776989296</v>
+        <v>1.1495894495004899</v>
       </c>
       <c r="E81" s="2">
-        <v>4.3949133500027502</v>
+        <v>1.15154410550167</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>3073</v>
+        <v>810</v>
       </c>
       <c r="B82">
-        <v>4.3934037495062501</v>
+        <v>1.1500664430015599</v>
       </c>
       <c r="C82">
-        <v>4.3853470613022996</v>
+        <v>1.1488096974964701</v>
       </c>
       <c r="D82" s="2">
-        <v>4.3859115923023602</v>
+        <v>1.14873579270351</v>
       </c>
       <c r="E82" s="2">
-        <v>4.3953194876012196</v>
+        <v>1.1515921852973401</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>3156</v>
+        <v>820</v>
       </c>
       <c r="B83">
-        <v>4.6253574120979399</v>
+        <v>1.1505305351980399</v>
       </c>
       <c r="C83">
-        <v>4.6190958194034399</v>
+        <v>1.14919286380609</v>
       </c>
       <c r="D83" s="2">
-        <v>4.61688279299924</v>
+        <v>1.1488694032042901</v>
       </c>
       <c r="E83" s="2">
-        <v>4.6287809478970301</v>
+        <v>1.15157967220002</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>3239</v>
+        <v>830</v>
       </c>
       <c r="B84">
-        <v>4.6242938347939297</v>
+        <v>1.3796782727004</v>
       </c>
       <c r="C84">
-        <v>4.6157836322919996</v>
+        <v>1.3785449532020699</v>
       </c>
       <c r="D84" s="2">
-        <v>4.6167181064934901</v>
+        <v>1.3785754157040999</v>
       </c>
       <c r="E84" s="2">
-        <v>4.6258708813016698</v>
+        <v>1.38150272549683</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85">
+        <v>840</v>
+      </c>
+      <c r="B85">
+        <v>1.3815889511941299</v>
+      </c>
+      <c r="C85">
+        <v>1.38072179710288</v>
+      </c>
+      <c r="D85" s="2">
+        <v>1.3806599286035599</v>
+      </c>
+      <c r="E85" s="2">
+        <v>1.3830144133040401</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>850</v>
+      </c>
+      <c r="B86">
+        <v>1.38037984969851</v>
+      </c>
+      <c r="C86">
+        <v>1.37911302110587</v>
+      </c>
+      <c r="D86" s="2">
+        <v>1.3793422223912699</v>
+      </c>
+      <c r="E86" s="2">
+        <v>1.3821519539007501</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>860</v>
+      </c>
+      <c r="B87">
+        <v>1.3797283040024899</v>
+      </c>
+      <c r="C87">
+        <v>1.3787791148017201</v>
+      </c>
+      <c r="D87" s="2">
+        <v>1.37845527309691</v>
+      </c>
+      <c r="E87" s="2">
+        <v>1.38160211200738</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>870</v>
+      </c>
+      <c r="B88">
+        <v>1.38849876999884</v>
+      </c>
+      <c r="C88">
+        <v>1.38704117750166</v>
+      </c>
+      <c r="D88" s="2">
+        <v>1.38845811379287</v>
+      </c>
+      <c r="E88" s="2">
+        <v>1.3900572519021801</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>880</v>
+      </c>
+      <c r="B89">
+        <v>1.37939181109977</v>
+      </c>
+      <c r="C89">
+        <v>1.37802767610119</v>
+      </c>
+      <c r="D89" s="2">
+        <v>1.3781997638056001</v>
+      </c>
+      <c r="E89" s="2">
+        <v>1.38105860389623</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>890</v>
+      </c>
+      <c r="B90">
+        <v>1.3794358067083501</v>
+      </c>
+      <c r="C90">
+        <v>1.3780890883921499</v>
+      </c>
+      <c r="D90" s="2">
+        <v>1.3781623007991499</v>
+      </c>
+      <c r="E90" s="2">
+        <v>1.3810778347979</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>900</v>
+      </c>
+      <c r="B91">
+        <v>1.3797102640950401</v>
+      </c>
+      <c r="C91">
+        <v>1.37836480040277</v>
+      </c>
+      <c r="D91" s="2">
+        <v>1.37826375950389</v>
+      </c>
+      <c r="E91" s="2">
+        <v>1.38215582139528</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>910</v>
+      </c>
+      <c r="B92">
+        <v>1.37931745040405</v>
+      </c>
+      <c r="C92">
+        <v>1.3777032031066401</v>
+      </c>
+      <c r="D92" s="2">
+        <v>1.3777681503983299</v>
+      </c>
+      <c r="E92" s="2">
+        <v>1.3806159703948599</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>920</v>
+      </c>
+      <c r="B93">
+        <v>1.3791915929948999</v>
+      </c>
+      <c r="C93">
+        <v>1.3777074908953999</v>
+      </c>
+      <c r="D93" s="2">
+        <v>1.3777150526991999</v>
+      </c>
+      <c r="E93" s="2">
+        <v>1.3806413364101899</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>930</v>
+      </c>
+      <c r="B94">
+        <v>1.3792114683936201</v>
+      </c>
+      <c r="C94">
+        <v>1.37768711639801</v>
+      </c>
+      <c r="D94" s="2">
+        <v>1.37766543469624</v>
+      </c>
+      <c r="E94" s="2">
+        <v>1.3806771277013401</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>940</v>
+      </c>
+      <c r="B95">
+        <v>1.3792617451996101</v>
+      </c>
+      <c r="C95">
+        <v>1.37761127970297</v>
+      </c>
+      <c r="D95" s="2">
+        <v>1.3776719874018399</v>
+      </c>
+      <c r="E95" s="2">
+        <v>1.38085108110535</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>950</v>
+      </c>
+      <c r="B96">
+        <v>1.3793482760025599</v>
+      </c>
+      <c r="C96">
+        <v>1.3777834555017701</v>
+      </c>
+      <c r="D96" s="2">
+        <v>1.37780253390083</v>
+      </c>
+      <c r="E96" s="2">
+        <v>1.3806859989010201</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>960</v>
+      </c>
+      <c r="B97">
+        <v>1.37938820869167</v>
+      </c>
+      <c r="C97">
+        <v>1.3777355083948299</v>
+      </c>
+      <c r="D97" s="2">
+        <v>1.37783118000224</v>
+      </c>
+      <c r="E97" s="2">
+        <v>1.38073047899233</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>970</v>
+      </c>
+      <c r="B98">
+        <v>1.37972648270661</v>
+      </c>
+      <c r="C98">
+        <v>1.3779501956028899</v>
+      </c>
+      <c r="D98" s="2">
+        <v>1.37803198599431</v>
+      </c>
+      <c r="E98" s="2">
+        <v>1.38087503030401</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>980</v>
+      </c>
+      <c r="B99">
+        <v>1.3794488236948299</v>
+      </c>
+      <c r="C99">
+        <v>1.37784946229803</v>
+      </c>
+      <c r="D99" s="2">
+        <v>1.3778431654980501</v>
+      </c>
+      <c r="E99" s="2">
+        <v>1.3808377706984101</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>990</v>
+      </c>
+      <c r="B100">
+        <v>1.3796682497079</v>
+      </c>
+      <c r="C100">
+        <v>1.37788613379962</v>
+      </c>
+      <c r="D100" s="2">
+        <v>1.3778851910014001</v>
+      </c>
+      <c r="E100" s="2">
+        <v>1.3810263734980199</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>1000</v>
+      </c>
+      <c r="B101">
+        <v>1.6089575650024901</v>
+      </c>
+      <c r="C101">
+        <v>1.6072365430008999</v>
+      </c>
+      <c r="D101" s="2">
+        <v>1.6072468711994501</v>
+      </c>
+      <c r="E101" s="2">
+        <v>1.6107258832998901</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>1010</v>
+      </c>
+      <c r="B102">
+        <v>1.6092892139044099</v>
+      </c>
+      <c r="C102">
+        <v>1.6075505720946199</v>
+      </c>
+      <c r="D102" s="2">
+        <v>1.60763564940571</v>
+      </c>
+      <c r="E102" s="2">
+        <v>1.61108786609984</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>1020</v>
+      </c>
+      <c r="B103">
+        <v>1.6091833823069399</v>
+      </c>
+      <c r="C103">
+        <v>1.60741165200161</v>
+      </c>
+      <c r="D103" s="2">
+        <v>1.6074102195983799</v>
+      </c>
+      <c r="E103" s="2">
+        <v>1.6110013935074601</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>1030</v>
+      </c>
+      <c r="B104">
+        <v>1.60921744930528</v>
+      </c>
+      <c r="C104">
+        <v>1.60739559020294</v>
+      </c>
+      <c r="D104" s="2">
+        <v>1.60741771490575</v>
+      </c>
+      <c r="E104" s="2">
+        <v>1.61111730379634</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>1040</v>
+      </c>
+      <c r="B105">
+        <v>1.6094024849066</v>
+      </c>
+      <c r="C105">
+        <v>1.60740231919189</v>
+      </c>
+      <c r="D105" s="2">
+        <v>1.6075019588985</v>
+      </c>
+      <c r="E105" s="2">
+        <v>1.6110319457045901</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>1050</v>
+      </c>
+      <c r="B106">
+        <v>1.6097251546961999</v>
+      </c>
+      <c r="C106">
+        <v>1.6079583671031199</v>
+      </c>
+      <c r="D106" s="2">
+        <v>1.60790537260036</v>
+      </c>
+      <c r="E106" s="2">
+        <v>1.61158625330426</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>1060</v>
+      </c>
+      <c r="B107">
+        <v>1.6101628741962399</v>
+      </c>
+      <c r="C107">
+        <v>1.60902784230711</v>
+      </c>
+      <c r="D107" s="2">
+        <v>1.6082944323992701</v>
+      </c>
+      <c r="E107" s="2">
+        <v>1.6118952353004701</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>1070</v>
+      </c>
+      <c r="B108">
+        <v>1.6171225512880401</v>
+      </c>
+      <c r="C108">
+        <v>1.61525499979761</v>
+      </c>
+      <c r="D108" s="2">
+        <v>1.6152748536042001</v>
+      </c>
+      <c r="E108" s="2">
+        <v>1.61877410019806</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>1080</v>
+      </c>
+      <c r="B109">
+        <v>1.6171386397996601</v>
+      </c>
+      <c r="C109">
+        <v>1.6152396510035001</v>
+      </c>
+      <c r="D109" s="2">
+        <v>1.6152735515002801</v>
+      </c>
+      <c r="E109" s="2">
+        <v>1.6187431423066301</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>1090</v>
+      </c>
+      <c r="B110">
+        <v>1.6171530411942501</v>
+      </c>
+      <c r="C110">
+        <v>1.6152129433990901</v>
+      </c>
+      <c r="D110" s="2">
+        <v>1.6152159998979101</v>
+      </c>
+      <c r="E110" s="2">
+        <v>1.6186979506019199</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>1100</v>
+      </c>
+      <c r="B111">
+        <v>1.60998642389604</v>
+      </c>
+      <c r="C111">
+        <v>1.6087797512984201</v>
+      </c>
+      <c r="D111" s="2">
+        <v>1.6083554270066001</v>
+      </c>
+      <c r="E111" s="2">
+        <v>1.6120198498960201</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>1110</v>
+      </c>
+      <c r="B112">
+        <v>1.60925144069333</v>
+      </c>
+      <c r="C112">
+        <v>1.6073679266046299</v>
+      </c>
+      <c r="D112" s="2">
+        <v>1.60739037789899</v>
+      </c>
+      <c r="E112" s="2">
+        <v>1.61099677579186</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>1120</v>
+      </c>
+      <c r="B113">
+        <v>1.60927227150095</v>
+      </c>
+      <c r="C113">
+        <v>1.6072540613036801</v>
+      </c>
+      <c r="D113" s="2">
+        <v>1.6072663729093599</v>
+      </c>
+      <c r="E113" s="2">
+        <v>1.6107454917044299</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>1130</v>
+      </c>
+      <c r="B114">
+        <v>1.6091902857879099</v>
+      </c>
+      <c r="C114">
+        <v>1.60718803769559</v>
+      </c>
+      <c r="D114" s="2">
+        <v>1.6071943958027901</v>
+      </c>
+      <c r="E114" s="2">
+        <v>1.6106684457015901</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>1140</v>
+      </c>
+      <c r="B115">
+        <v>1.6091090553018099</v>
+      </c>
+      <c r="C115">
+        <v>1.60711307370074</v>
+      </c>
+      <c r="D115" s="2">
+        <v>1.6071283737997799</v>
+      </c>
+      <c r="E115" s="2">
+        <v>1.6106479533977101</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>1150</v>
+      </c>
+      <c r="B116">
+        <v>1.60919322550907</v>
+      </c>
+      <c r="C116">
+        <v>1.6071171908944899</v>
+      </c>
+      <c r="D116" s="2">
+        <v>1.60716854659985</v>
+      </c>
+      <c r="E116" s="2">
+        <v>1.6106668275009699</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>1160</v>
+      </c>
+      <c r="B117">
+        <v>1.60924434079788</v>
+      </c>
+      <c r="C117">
+        <v>1.60717685879935</v>
+      </c>
+      <c r="D117" s="2">
+        <v>1.6072051581984801</v>
+      </c>
+      <c r="E117" s="2">
+        <v>1.6106280994048501</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>1170</v>
+      </c>
+      <c r="B118">
+        <v>1.83883663139276</v>
+      </c>
+      <c r="C118">
+        <v>1.8367576037009701</v>
+      </c>
+      <c r="D118" s="2">
+        <v>1.8368816780988699</v>
+      </c>
+      <c r="E118" s="2">
+        <v>1.8410144598033999</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>1180</v>
+      </c>
+      <c r="B119">
+        <v>1.8390819088992401</v>
+      </c>
+      <c r="C119">
+        <v>1.83749364090617</v>
+      </c>
+      <c r="D119" s="2">
+        <v>1.83702383260097</v>
+      </c>
+      <c r="E119" s="2">
+        <v>1.8411721535026999</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>1190</v>
+      </c>
+      <c r="B120">
+        <v>1.83900496900459</v>
+      </c>
+      <c r="C120">
+        <v>1.83690752830007</v>
+      </c>
+      <c r="D120" s="2">
+        <v>1.8368970511917699</v>
+      </c>
+      <c r="E120" s="2">
+        <v>1.84086367369745</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>1200</v>
+      </c>
+      <c r="B121">
+        <v>1.83946967689844</v>
+      </c>
+      <c r="C121">
+        <v>1.83766781939339</v>
+      </c>
+      <c r="D121" s="2">
+        <v>1.8373754205895201</v>
+      </c>
+      <c r="E121" s="2">
+        <v>1.8412736014041</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>1210</v>
+      </c>
+      <c r="B122">
+        <v>1.84603875949978</v>
+      </c>
+      <c r="C122">
+        <v>1.8443322145933001</v>
+      </c>
+      <c r="D122" s="2">
+        <v>1.8442933000013</v>
+      </c>
+      <c r="E122" s="2">
+        <v>1.8478392875898799</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>1220</v>
+      </c>
+      <c r="B123">
+        <v>1.8500633292904201</v>
+      </c>
+      <c r="C123">
+        <v>1.84731618220102</v>
+      </c>
+      <c r="D123" s="2">
+        <v>1.84743153159652</v>
+      </c>
+      <c r="E123" s="2">
+        <v>1.8514508187959999</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>1230</v>
+      </c>
+      <c r="B124">
+        <v>1.8487160576914901</v>
+      </c>
+      <c r="C124">
+        <v>1.8463182530962501</v>
+      </c>
+      <c r="D124" s="2">
+        <v>1.8462928061053301</v>
+      </c>
+      <c r="E124" s="2">
+        <v>1.85063735659641</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>1240</v>
+      </c>
+      <c r="B125">
+        <v>1.84853502680198</v>
+      </c>
+      <c r="C125">
+        <v>1.8462186326010801</v>
+      </c>
+      <c r="D125" s="2">
+        <v>1.8462350819987401</v>
+      </c>
+      <c r="E125" s="2">
+        <v>1.8502037377009399</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>1250</v>
+      </c>
+      <c r="B126">
+        <v>1.8483762653035201</v>
+      </c>
+      <c r="C126">
+        <v>1.8461304447089699</v>
+      </c>
+      <c r="D126" s="2">
+        <v>1.8461340495996399</v>
+      </c>
+      <c r="E126" s="2">
+        <v>1.8501216066943</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>1260</v>
+      </c>
+      <c r="B127">
+        <v>1.84881075349694</v>
+      </c>
+      <c r="C127">
+        <v>1.8464708091108999</v>
+      </c>
+      <c r="D127" s="2">
+        <v>1.84651371580112</v>
+      </c>
+      <c r="E127" s="2">
+        <v>1.8504632306998201</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>1270</v>
+      </c>
+      <c r="B128">
+        <v>1.8483164633013001</v>
+      </c>
+      <c r="C128">
+        <v>1.8459961700064</v>
+      </c>
+      <c r="D128" s="2">
+        <v>1.84602536869933</v>
+      </c>
+      <c r="E128" s="2">
+        <v>1.8499897633009801</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>1280</v>
+      </c>
+      <c r="B129">
+        <v>1.8484433067977</v>
+      </c>
+      <c r="C129">
+        <v>1.84612269129575</v>
+      </c>
+      <c r="D129" s="2">
+        <v>1.8460723425989201</v>
+      </c>
+      <c r="E129" s="2">
+        <v>1.8504252972998001</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>1290</v>
+      </c>
+      <c r="B130">
+        <v>1.8484967579046401</v>
+      </c>
+      <c r="C130">
+        <v>1.84616369479917</v>
+      </c>
+      <c r="D130" s="2">
+        <v>1.8461990632029399</v>
+      </c>
+      <c r="E130" s="2">
+        <v>1.8500944181025201</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>1300</v>
+      </c>
+      <c r="B131">
+        <v>1.84860940560029</v>
+      </c>
+      <c r="C131">
+        <v>1.8463498634984701</v>
+      </c>
+      <c r="D131" s="2">
+        <v>1.8462655576920901</v>
+      </c>
+      <c r="E131" s="2">
+        <v>1.85023737369774</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>1310</v>
+      </c>
+      <c r="B132">
+        <v>1.84860542670649</v>
+      </c>
+      <c r="C132">
+        <v>1.8462207815056899</v>
+      </c>
+      <c r="D132" s="2">
+        <v>1.84620803619473</v>
+      </c>
+      <c r="E132" s="2">
+        <v>1.85021976959251</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>1320</v>
+      </c>
+      <c r="B133">
+        <v>1.84877236701286</v>
+      </c>
+      <c r="C133">
+        <v>1.84630793029791</v>
+      </c>
+      <c r="D133" s="2">
+        <v>1.8462177954002901</v>
+      </c>
+      <c r="E133" s="2">
+        <v>1.85032236030237</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>1330</v>
+      </c>
+      <c r="B134">
+        <v>2.0796010954087198</v>
+      </c>
+      <c r="C134">
+        <v>2.0771461598938901</v>
+      </c>
+      <c r="D134" s="2">
+        <v>2.0771728569932701</v>
+      </c>
+      <c r="E134" s="2">
+        <v>2.0816448420067899</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>1340</v>
+      </c>
+      <c r="B135">
+        <v>2.0795705691023598</v>
+      </c>
+      <c r="C135">
+        <v>2.0768764104024702</v>
+      </c>
+      <c r="D135" s="2">
+        <v>2.0768966904070099</v>
+      </c>
+      <c r="E135" s="2">
+        <v>2.0812629579901101</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>1350</v>
+      </c>
+      <c r="B136">
+        <v>2.0793187164992499</v>
+      </c>
+      <c r="C136">
+        <v>2.07677837179217</v>
+      </c>
+      <c r="D136" s="2">
+        <v>2.07684967440145</v>
+      </c>
+      <c r="E136" s="2">
+        <v>2.0813091366930099</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>1360</v>
+      </c>
+      <c r="B137">
+        <v>2.0795250945055099</v>
+      </c>
+      <c r="C137">
+        <v>2.0770592743938301</v>
+      </c>
+      <c r="D137" s="2">
+        <v>2.0770350880993602</v>
+      </c>
+      <c r="E137" s="2">
+        <v>2.08148447619751</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>1370</v>
+      </c>
+      <c r="B138">
+        <v>2.0793809257040201</v>
+      </c>
+      <c r="C138">
+        <v>2.0767809055003399</v>
+      </c>
+      <c r="D138" s="2">
+        <v>2.0768281766941001</v>
+      </c>
+      <c r="E138" s="2">
+        <v>2.0813141265025399</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>1380</v>
+      </c>
+      <c r="B139">
+        <v>2.0794153880036901</v>
+      </c>
+      <c r="C139">
+        <v>2.0767911534130601</v>
+      </c>
+      <c r="D139" s="2">
+        <v>2.0768460754945401</v>
+      </c>
+      <c r="E139" s="2">
+        <v>2.0812983006908299</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>1390</v>
+      </c>
+      <c r="B140">
+        <v>2.07965755159384</v>
+      </c>
+      <c r="C140">
+        <v>2.0770082395014402</v>
+      </c>
+      <c r="D140" s="2">
+        <v>2.07702341709664</v>
+      </c>
+      <c r="E140" s="2">
+        <v>2.0817456145043201</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>1400</v>
+      </c>
+      <c r="B141">
+        <v>2.0794823887976199</v>
+      </c>
+      <c r="C141">
+        <v>2.0769020565086902</v>
+      </c>
+      <c r="D141" s="2">
+        <v>2.0768399006061302</v>
+      </c>
+      <c r="E141" s="2">
+        <v>2.0813249490980499</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>1410</v>
+      </c>
+      <c r="B142">
+        <v>2.0802576194037101</v>
+      </c>
+      <c r="C142">
+        <v>2.0783350421930602</v>
+      </c>
+      <c r="D142" s="2">
+        <v>2.07811150330526</v>
+      </c>
+      <c r="E142" s="2">
+        <v>2.0822869486073601</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>1496</v>
+      </c>
+      <c r="B143">
+        <v>2.3111542399994498</v>
+      </c>
+      <c r="C143">
+        <v>2.3087513166989</v>
+      </c>
+      <c r="D143" s="2">
+        <v>2.3078786508980502</v>
+      </c>
+      <c r="E143" s="2">
+        <v>2.3142482793002199</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>1579</v>
+      </c>
+      <c r="B144">
+        <v>2.3117302255002801</v>
+      </c>
+      <c r="C144">
+        <v>2.30820002760119</v>
+      </c>
+      <c r="D144" s="2">
+        <v>2.3088033395000802</v>
+      </c>
+      <c r="E144" s="2">
+        <v>2.3128195776003801</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>1662</v>
+      </c>
+      <c r="B145">
+        <v>2.54227149650105</v>
+      </c>
+      <c r="C145">
+        <v>2.5392136873990201</v>
+      </c>
+      <c r="D145" s="2">
+        <v>2.5397528821984401</v>
+      </c>
+      <c r="E145" s="2">
+        <v>2.5442274139004399</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>1745</v>
+      </c>
+      <c r="B146">
+        <v>2.5428949605011399</v>
+      </c>
+      <c r="C146">
+        <v>2.53902974829579</v>
+      </c>
+      <c r="D146" s="2">
+        <v>2.5400896978004299</v>
+      </c>
+      <c r="E146" s="2">
+        <v>2.5443249798015999</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>1828</v>
+      </c>
+      <c r="B147">
+        <v>2.7741687695033699</v>
+      </c>
+      <c r="C147">
+        <v>2.7699574161993898</v>
+      </c>
+      <c r="D147" s="2">
+        <v>2.7708509844003801</v>
+      </c>
+      <c r="E147" s="2">
+        <v>2.7758213149019801</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>1911</v>
+      </c>
+      <c r="B148">
+        <v>2.77523935579993</v>
+      </c>
+      <c r="C148">
+        <v>2.7703980756989002</v>
+      </c>
+      <c r="D148" s="2">
+        <v>2.77003198079837</v>
+      </c>
+      <c r="E148" s="2">
+        <v>2.77650629879972</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>1994</v>
+      </c>
+      <c r="B149">
+        <v>3.0064893082006101</v>
+      </c>
+      <c r="C149">
+        <v>3.0019949998019002</v>
+      </c>
+      <c r="D149" s="2">
+        <v>3.0010721826023601</v>
+      </c>
+      <c r="E149" s="2">
+        <v>3.0074823880975599</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>2077</v>
+      </c>
+      <c r="B150">
+        <v>3.0047839199989501</v>
+      </c>
+      <c r="C150">
+        <v>3.0005700640020199</v>
+      </c>
+      <c r="D150" s="2">
+        <v>3.00135763599901</v>
+      </c>
+      <c r="E150" s="2">
+        <v>3.0072964612987501</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>2160</v>
+      </c>
+      <c r="B151">
+        <v>3.2354625024003298</v>
+      </c>
+      <c r="C151">
+        <v>3.2312648426006398</v>
+      </c>
+      <c r="D151" s="2">
+        <v>3.2317017569992399</v>
+      </c>
+      <c r="E151" s="2">
+        <v>3.23821297069916</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>2243</v>
+      </c>
+      <c r="B152">
+        <v>3.22337480519854</v>
+      </c>
+      <c r="C152">
+        <v>3.2188382781001499</v>
+      </c>
+      <c r="D152" s="2">
+        <v>3.2185373202999399</v>
+      </c>
+      <c r="E152" s="2">
+        <v>3.2266523780042902</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>2326</v>
+      </c>
+      <c r="B153">
+        <v>3.4530660588028601</v>
+      </c>
+      <c r="C153">
+        <v>3.4469978186021701</v>
+      </c>
+      <c r="D153" s="2">
+        <v>3.4468672844988699</v>
+      </c>
+      <c r="E153" s="2">
+        <v>3.4548454540021298</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>2409</v>
+      </c>
+      <c r="B154">
+        <v>3.45246772610116</v>
+      </c>
+      <c r="C154">
+        <v>3.4471679462021698</v>
+      </c>
+      <c r="D154" s="2">
+        <v>3.4486230679009102</v>
+      </c>
+      <c r="E154" s="2">
+        <v>3.4544709747977298</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>2492</v>
+      </c>
+      <c r="B155">
+        <v>3.68389598089815</v>
+      </c>
+      <c r="C155">
+        <v>3.6775013342004899</v>
+      </c>
+      <c r="D155" s="2">
+        <v>3.6784485956992201</v>
+      </c>
+      <c r="E155" s="2">
+        <v>3.6863269559984402</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>2575</v>
+      </c>
+      <c r="B156">
+        <v>3.6827995692001401</v>
+      </c>
+      <c r="C156">
+        <v>3.6775139375986301</v>
+      </c>
+      <c r="D156" s="2">
+        <v>3.6774336517009898</v>
+      </c>
+      <c r="E156" s="2">
+        <v>3.68622713070144</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>2658</v>
+      </c>
+      <c r="B157">
+        <v>3.9125397755018598</v>
+      </c>
+      <c r="C157">
+        <v>3.9069434099015701</v>
+      </c>
+      <c r="D157" s="2">
+        <v>3.9071265521011802</v>
+      </c>
+      <c r="E157" s="2">
+        <v>3.9152474940019601</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>2741</v>
+      </c>
+      <c r="B158">
+        <v>3.9134088366976298</v>
+      </c>
+      <c r="C158">
+        <v>3.9071483164032501</v>
+      </c>
+      <c r="D158" s="2">
+        <v>3.9076248787019701</v>
+      </c>
+      <c r="E158" s="2">
+        <v>3.9154213372996298</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>2824</v>
+      </c>
+      <c r="B159">
+        <v>4.14514273610075</v>
+      </c>
+      <c r="C159">
+        <v>4.13869946940176</v>
+      </c>
+      <c r="D159" s="2">
+        <v>4.1380854752973297</v>
+      </c>
+      <c r="E159" s="2">
+        <v>4.1484387924985597</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>2907</v>
+      </c>
+      <c r="B160">
+        <v>4.16121216540341</v>
+      </c>
+      <c r="C160">
+        <v>4.1553411544995402</v>
+      </c>
+      <c r="D160" s="2">
+        <v>4.1548015606029303</v>
+      </c>
+      <c r="E160" s="2">
+        <v>4.1654067057992501</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>2990</v>
+      </c>
+      <c r="B161">
+        <v>4.3926759652978902</v>
+      </c>
+      <c r="C161">
+        <v>4.3864021097011499</v>
+      </c>
+      <c r="D161" s="2">
+        <v>4.3859517776989296</v>
+      </c>
+      <c r="E161" s="2">
+        <v>4.3949133500027502</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>3073</v>
+      </c>
+      <c r="B162">
+        <v>4.3934037495062501</v>
+      </c>
+      <c r="C162">
+        <v>4.3853470613022996</v>
+      </c>
+      <c r="D162" s="2">
+        <v>4.3859115923023602</v>
+      </c>
+      <c r="E162" s="2">
+        <v>4.3953194876012196</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>3156</v>
+      </c>
+      <c r="B163">
+        <v>4.6253574120979399</v>
+      </c>
+      <c r="C163">
+        <v>4.6190958194034399</v>
+      </c>
+      <c r="D163" s="2">
+        <v>4.61688279299924</v>
+      </c>
+      <c r="E163" s="2">
+        <v>4.6287809478970301</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>3239</v>
+      </c>
+      <c r="B164">
+        <v>4.6242938347939297</v>
+      </c>
+      <c r="C164">
+        <v>4.6157836322919996</v>
+      </c>
+      <c r="D164" s="2">
+        <v>4.6167181064934901</v>
+      </c>
+      <c r="E164" s="2">
+        <v>4.6258708813016698</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A165">
         <v>3322</v>
       </c>
-      <c r="B85">
+      <c r="B165">
         <v>4.8561269555982998</v>
       </c>
-      <c r="C85">
+      <c r="C165">
         <v>4.8499624816984497</v>
       </c>
-      <c r="D85" s="2">
+      <c r="D165" s="2">
         <v>4.8485004974027097</v>
       </c>
-      <c r="E85" s="2">
+      <c r="E165" s="2">
         <v>4.8606518181935803</v>
       </c>
     </row>
@@ -24960,7 +26320,7 @@
   <dimension ref="A1:K258"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30907,1000 +32267,1020 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>10</v>
-      </c>
-      <c r="B1">
-        <v>2.1690967601898498E-2</v>
-      </c>
-      <c r="C1">
-        <v>1.37157142989963E-2</v>
-      </c>
-      <c r="D1">
-        <v>2.0314045699342299E-2</v>
-      </c>
-      <c r="E1">
-        <v>3.1167784999888599E-2</v>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B2">
-        <v>2.2036971800298399E-2</v>
+        <v>0.18137247870436099</v>
       </c>
       <c r="C2">
-        <v>1.3661996401060601E-2</v>
-      </c>
-      <c r="D2">
-        <v>2.06752309988587E-2</v>
-      </c>
-      <c r="E2">
-        <v>3.1999148599243202E-2</v>
+        <v>0.114551344609571</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.16540585369857499</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.26464184719334299</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B3">
-        <v>2.26507690007565E-2</v>
+        <v>0.178177898299509</v>
       </c>
       <c r="C3">
-        <v>1.4258930000141799E-2</v>
-      </c>
-      <c r="D3">
-        <v>1.98071789012828E-2</v>
-      </c>
-      <c r="E3">
-        <v>3.3257645398953102E-2</v>
+        <v>0.113612802905845</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.16403479089731199</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.26190727809480402</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B4">
-        <v>2.3847526999997998E-2</v>
+        <v>0.18125109710126699</v>
       </c>
       <c r="C4">
-        <v>1.4869628599444599E-2</v>
-      </c>
-      <c r="D4">
-        <v>2.1024842300357699E-2</v>
-      </c>
-      <c r="E4">
-        <v>3.49881900010586E-2</v>
+        <v>0.115019513498737</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.16476123260144901</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.267763427402678</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B5">
-        <v>2.5519760200222601E-2</v>
+        <v>0.19064662419950701</v>
       </c>
       <c r="C5">
-        <v>1.58363511993229E-2</v>
-      </c>
-      <c r="D5">
-        <v>2.1506781699281399E-2</v>
-      </c>
-      <c r="E5">
-        <v>3.76376413989419E-2</v>
+        <v>0.11972386819998</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.17070820380049501</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.28270401759927999</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B6">
-        <v>2.7691572999537999E-2</v>
+        <v>0.197864628702518</v>
       </c>
       <c r="C6">
-        <v>1.69724583014613E-2</v>
-      </c>
-      <c r="D6">
-        <v>2.4698843399892201E-2</v>
-      </c>
-      <c r="E6">
-        <v>4.0856473599887901E-2</v>
+        <v>0.123736933201143</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.164118085800873</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.29330546089986398</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B7">
-        <v>2.9095443799815199E-2</v>
+        <v>0.209717707601703</v>
       </c>
       <c r="C7">
-        <v>1.7757015300230699E-2</v>
-      </c>
-      <c r="D7">
-        <v>2.3964384300415899E-2</v>
-      </c>
-      <c r="E7">
-        <v>4.2983620199083798E-2</v>
+        <v>0.130933015299524</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.18157307090059399</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.312148551298014</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B8">
-        <v>3.0552121400069101E-2</v>
+        <v>0.218559509799888</v>
       </c>
       <c r="C8">
-        <v>1.8662295300237001E-2</v>
-      </c>
-      <c r="D8">
-        <v>2.3889265301295301E-2</v>
-      </c>
-      <c r="E8">
-        <v>4.5209344399154298E-2</v>
+        <v>0.134299072901922</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.181143911600156</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.32534623589926898</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B9">
-        <v>3.0599256000823499E-2</v>
+        <v>0.22929859209980299</v>
       </c>
       <c r="C9">
-        <v>1.84602594996249E-2</v>
-      </c>
-      <c r="D9">
-        <v>2.7137128299545999E-2</v>
-      </c>
-      <c r="E9">
-        <v>4.5112074701137303E-2</v>
+        <v>0.13998675250131701</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.17922173230053801</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.34166566859803399</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B10">
-        <v>3.4717165000438401E-2</v>
+        <v>0.24036286729842599</v>
       </c>
       <c r="C10">
-        <v>2.09461496002404E-2</v>
-      </c>
-      <c r="D10">
-        <v>2.4089805200492202E-2</v>
-      </c>
-      <c r="E10">
-        <v>5.14824370993665E-2</v>
+        <v>0.14492907279745801</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.197688863500116</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.35807708449956399</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B11">
-        <v>3.3465308699487599E-2</v>
+        <v>0.25079963459938798</v>
       </c>
       <c r="C11">
-        <v>1.9911103999947902E-2</v>
-      </c>
-      <c r="D11">
-        <v>2.7051253599893198E-2</v>
-      </c>
-      <c r="E11">
-        <v>4.9634584999330399E-2</v>
+        <v>0.15057349700109601</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.19221845590181999</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.37412899729806598</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B12">
-        <v>3.8299250899581201E-2</v>
+        <v>0.26509511920194201</v>
       </c>
       <c r="C12">
-        <v>2.2735391799869799E-2</v>
-      </c>
-      <c r="D12">
-        <v>2.9347514600522099E-2</v>
-      </c>
-      <c r="E12">
-        <v>5.6951784800185097E-2</v>
+        <v>0.15755791049832599</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.199032337298922</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.39508336970247898</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B13">
-        <v>4.30362540006171E-2</v>
+        <v>0.28070784589890502</v>
       </c>
       <c r="C13">
-        <v>2.52301566002643E-2</v>
-      </c>
-      <c r="D13">
-        <v>3.0964612099341999E-2</v>
-      </c>
-      <c r="E13">
-        <v>6.4050917999338694E-2</v>
+        <v>0.16525435260027699</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.223382452200166</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.418769063498803</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B14">
-        <v>3.85496387993043E-2</v>
+        <v>0.29447514059993402</v>
       </c>
       <c r="C14">
-        <v>2.2572279099949799E-2</v>
-      </c>
-      <c r="D14">
-        <v>2.8171360199485199E-2</v>
-      </c>
-      <c r="E14">
-        <v>5.7229245700546001E-2</v>
+        <v>0.17318396870050401</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.20776454909882799</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.439293220701438</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B15">
-        <v>4.3929768399539097E-2</v>
+        <v>0.30944367810025097</v>
       </c>
       <c r="C15">
-        <v>2.54802796000149E-2</v>
-      </c>
-      <c r="D15">
-        <v>3.1338234600116199E-2</v>
-      </c>
-      <c r="E15">
-        <v>6.5262794899717799E-2</v>
+        <v>0.18110131500034099</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.226737439300632</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.46238902359946199</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B16">
-        <v>4.9062909599888301E-2</v>
+        <v>0.32932741169970497</v>
       </c>
       <c r="C16">
-        <v>2.8358926600049E-2</v>
-      </c>
-      <c r="D16">
-        <v>3.5126203000254402E-2</v>
-      </c>
-      <c r="E16">
-        <v>7.2882102199400806E-2</v>
+        <v>0.19094976870001101</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.24674802769986801</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.49108377480042598</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B17">
-        <v>5.3451567499905601E-2</v>
+        <v>0.34237286469888201</v>
       </c>
       <c r="C17">
-        <v>3.1043678700188999E-2</v>
-      </c>
-      <c r="D17">
-        <v>3.75892175996341E-2</v>
-      </c>
-      <c r="E17">
-        <v>7.9614472399407499E-2</v>
+        <v>0.19563397660022</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.25423380090051001</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.51208465109739298</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B18">
-        <v>5.9725946400430899E-2</v>
+        <v>0.35889004280070302</v>
       </c>
       <c r="C18">
-        <v>3.4180365500287697E-2</v>
-      </c>
-      <c r="D18">
-        <v>4.2102680799143803E-2</v>
-      </c>
-      <c r="E18">
-        <v>8.8607171100011303E-2</v>
+        <v>0.207360821401016</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.25349778650106602</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.53681810949947195</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B19">
-        <v>4.9158554799396299E-2</v>
+        <v>0.38557675460142399</v>
       </c>
       <c r="C19">
-        <v>2.7850497099643601E-2</v>
-      </c>
-      <c r="D19">
-        <v>3.7867709799502297E-2</v>
-      </c>
-      <c r="E19">
-        <v>7.3404659700099698E-2</v>
+        <v>0.22235246210020701</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.26658830179858301</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.57631603530116904</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B20">
-        <v>5.4185155599952801E-2</v>
+        <v>0.392913169801067</v>
       </c>
       <c r="C20">
-        <v>3.0617993699888699E-2</v>
-      </c>
-      <c r="D20">
-        <v>3.6349147000692E-2</v>
-      </c>
-      <c r="E20">
-        <v>8.05842926001787E-2</v>
+        <v>0.22081824339929801</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.28057265940224102</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.58813770830001799</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B21">
-        <v>5.9884829700604297E-2</v>
+        <v>0.41349738149910897</v>
       </c>
       <c r="C21">
-        <v>3.3557708100124699E-2</v>
-      </c>
-      <c r="D21">
-        <v>3.8694037299865099E-2</v>
-      </c>
-      <c r="E21">
-        <v>8.8785371800258805E-2</v>
+        <v>0.23329991930022501</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.29194217570165998</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.618575424000118</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B22">
-        <v>6.5675185900363406E-2</v>
+        <v>0.43601635569903002</v>
       </c>
       <c r="C22">
-        <v>3.6774284500825101E-2</v>
-      </c>
-      <c r="D22">
-        <v>4.3876089699733702E-2</v>
-      </c>
-      <c r="E22">
-        <v>9.7442488399974506E-2</v>
+        <v>0.24566208319847599</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.29590614290009398</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.65267895890119598</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B23">
-        <v>7.2057334399505596E-2</v>
+        <v>0.45636643769903401</v>
       </c>
       <c r="C23">
-        <v>3.9862794499458599E-2</v>
-      </c>
-      <c r="D23">
-        <v>4.6277083599852602E-2</v>
-      </c>
-      <c r="E23">
-        <v>0.107445091900081</v>
+        <v>0.25714175649954901</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.321606210998652</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.68296276089895402</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B24">
-        <v>7.7537030499843201E-2</v>
+        <v>0.489594670701262</v>
       </c>
       <c r="C24">
-        <v>4.32175418998667E-2</v>
-      </c>
-      <c r="D24">
-        <v>4.9005559500619703E-2</v>
-      </c>
-      <c r="E24">
-        <v>0.116242364200297</v>
+        <v>0.27438167090021998</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.33116990489852399</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.73380018929892599</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B25">
-        <v>8.5213316000226705E-2</v>
+        <v>0.50425786460091304</v>
       </c>
       <c r="C25">
-        <v>4.64553530997363E-2</v>
-      </c>
-      <c r="D25">
-        <v>5.6818083800135297E-2</v>
-      </c>
-      <c r="E25">
-        <v>0.126418340699638</v>
+        <v>0.28152646279995602</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.32575381350106902</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.75532402740009197</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B26">
-        <v>9.2285688799711302E-2</v>
+        <v>0.53578460760036195</v>
       </c>
       <c r="C26">
-        <v>5.0893525099854703E-2</v>
-      </c>
-      <c r="D26">
-        <v>5.46305364005093E-2</v>
-      </c>
-      <c r="E26">
-        <v>0.137902797900642</v>
+        <v>0.29625182030122199</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.36256387859975803</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.80137029009965699</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B27">
-        <v>9.9676783400718699E-2</v>
+        <v>0.55243134469965205</v>
       </c>
       <c r="C27">
-        <v>5.4685993599196001E-2</v>
-      </c>
-      <c r="D27">
-        <v>6.5541299199685404E-2</v>
-      </c>
-      <c r="E27">
-        <v>0.149017001499305</v>
+        <v>0.30529929809981599</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.35888814459940399</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.82767463439940903</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B28">
-        <v>0.106782052400376</v>
+        <v>0.56386225130063305</v>
       </c>
       <c r="C28">
-        <v>5.8593675099837102E-2</v>
-      </c>
-      <c r="D28">
-        <v>6.4274385999669906E-2</v>
-      </c>
-      <c r="E28">
-        <v>0.15887331330013599</v>
+        <v>0.31020288049949102</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.35349783060009898</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0.84427593889922703</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B29">
-        <v>7.6985366099506694E-2</v>
+        <v>0.60219846310119396</v>
       </c>
       <c r="C29">
-        <v>4.1852644300524801E-2</v>
-      </c>
-      <c r="D29">
-        <v>5.35686781997355E-2</v>
-      </c>
-      <c r="E29">
-        <v>0.11425892220013301</v>
+        <v>0.33117907510077199</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.37323069640005901</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.90269752730037001</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B30">
-        <v>8.3042329300223997E-2</v>
+        <v>0.61024960029935704</v>
       </c>
       <c r="C30">
-        <v>4.4921706300010501E-2</v>
-      </c>
-      <c r="D30">
-        <v>5.0658609399943003E-2</v>
-      </c>
-      <c r="E30">
-        <v>0.12412737450013001</v>
+        <v>0.334577132199956</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.388531484500163</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0.91521942570070602</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B31">
-        <v>9.0261658899544198E-2</v>
+        <v>0.66170761520061205</v>
       </c>
       <c r="C31">
-        <v>4.8396229100399001E-2</v>
-      </c>
-      <c r="D31">
-        <v>5.8089980199838402E-2</v>
-      </c>
-      <c r="E31">
-        <v>0.13464656180039999</v>
+        <v>0.36079381510044101</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.415685907800252</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0.99140507830124902</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B32">
-        <v>9.6721036200324295E-2</v>
+        <v>0.67249862070002497</v>
       </c>
       <c r="C32">
-        <v>5.1910589800718297E-2</v>
-      </c>
-      <c r="D32">
-        <v>6.0760539100192502E-2</v>
-      </c>
-      <c r="E32">
-        <v>0.14372878490066701</v>
+        <v>0.36445291349991699</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.41598880939927702</v>
+      </c>
+      <c r="E32" s="2">
+        <v>1.0051012428013499</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B33">
-        <v>0.10383470519973299</v>
+        <v>0.72200017460072496</v>
       </c>
       <c r="C33">
-        <v>5.5878708100317399E-2</v>
-      </c>
-      <c r="D33">
-        <v>6.3057893000404805E-2</v>
-      </c>
-      <c r="E33">
-        <v>0.15478549430008501</v>
+        <v>0.39217183980035702</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.44254234730178699</v>
+      </c>
+      <c r="E33" s="2">
+        <v>1.0842629224003699</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B34">
-        <v>0.11058979850022201</v>
+        <v>0.77619038849952604</v>
       </c>
       <c r="C34">
-        <v>5.9623926700260198E-2</v>
-      </c>
-      <c r="D34">
-        <v>6.7316899299657895E-2</v>
-      </c>
-      <c r="E34">
-        <v>0.165755912399799</v>
+        <v>0.417664459400657</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.46370074589849503</v>
+      </c>
+      <c r="E34" s="2">
+        <v>1.15951763369848</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="B35">
-        <v>0.119162692299505</v>
+        <v>0.77435682380146298</v>
       </c>
       <c r="C35">
-        <v>6.3545805900321203E-2</v>
-      </c>
-      <c r="D35">
-        <v>7.1757024900398397E-2</v>
-      </c>
-      <c r="E35">
-        <v>0.17732238959997601</v>
+        <v>0.41766004430010001</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.481202615400252</v>
+      </c>
+      <c r="E35" s="2">
+        <v>1.1599023611994199</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B36">
-        <v>0.126665962700099</v>
+        <v>0.83002539730096003</v>
       </c>
       <c r="C36">
-        <v>6.7971004000173696E-2</v>
-      </c>
-      <c r="D36">
-        <v>7.8322140400450699E-2</v>
-      </c>
-      <c r="E36">
-        <v>0.18940161210011799</v>
+        <v>0.44497831310109098</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.50911448599981601</v>
+      </c>
+      <c r="E36" s="2">
+        <v>1.24210358429882</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B37">
-        <v>0.13584720089966101</v>
+        <v>0.82262723899857504</v>
       </c>
       <c r="C37">
-        <v>7.2834334600156495E-2</v>
-      </c>
-      <c r="D37">
-        <v>8.0123737099529496E-2</v>
-      </c>
-      <c r="E37">
-        <v>0.20233419899996</v>
+        <v>0.43957813800079698</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.50421253860022197</v>
+      </c>
+      <c r="E37" s="2">
+        <v>1.2311233212996699</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B38">
-        <v>0.14397692499987799</v>
+        <v>0.87879169659954603</v>
       </c>
       <c r="C38">
-        <v>7.6737041999694999E-2</v>
-      </c>
-      <c r="D38">
-        <v>8.3869877800134399E-2</v>
-      </c>
-      <c r="E38">
-        <v>0.21542801380055601</v>
+        <v>0.46826089119949699</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.53977741989783601</v>
+      </c>
+      <c r="E38" s="2">
+        <v>1.3173998277003101</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B39">
-        <v>0.15157367910032901</v>
+        <v>0.93047633260066498</v>
       </c>
       <c r="C39">
-        <v>8.0442921799840403E-2</v>
-      </c>
-      <c r="D39">
-        <v>8.9496370000415396E-2</v>
-      </c>
-      <c r="E39">
-        <v>0.226151120899521</v>
+        <v>0.49798612320028002</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.55602831089927296</v>
+      </c>
+      <c r="E39" s="2">
+        <v>1.3942098551991799</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B40">
-        <v>0.162014939600157</v>
+        <v>0.92494390499996304</v>
       </c>
       <c r="C40">
-        <v>8.5982456000056107E-2</v>
-      </c>
-      <c r="D40">
-        <v>9.6479982299933903E-2</v>
-      </c>
-      <c r="E40">
-        <v>0.243229428499944</v>
+        <v>0.49180204770018399</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0.547467828400658</v>
+      </c>
+      <c r="E40" s="2">
+        <v>1.3834212922009099</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B41">
-        <v>0.173671389200171</v>
+        <v>0.97271655060121698</v>
       </c>
       <c r="C41">
-        <v>9.2070981200231397E-2</v>
-      </c>
-      <c r="D41">
-        <v>9.9542085600296495E-2</v>
-      </c>
-      <c r="E41">
-        <v>0.260009983200507</v>
+        <v>0.52001140389893397</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.58294914270045395</v>
+      </c>
+      <c r="E41" s="2">
+        <v>1.4591394580995201</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B42">
-        <v>0.183437008199689</v>
+        <v>1.04640574590193</v>
       </c>
       <c r="C42">
-        <v>9.6989633899102007E-2</v>
-      </c>
-      <c r="D42">
-        <v>0.10827388910038201</v>
-      </c>
-      <c r="E42">
-        <v>0.273938244900091</v>
+        <v>0.55407663679980002</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.61040938389978605</v>
+      </c>
+      <c r="E42" s="2">
+        <v>1.5658393541003499</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B43">
-        <v>0.19478111089956601</v>
+        <v>1.09913228160021</v>
       </c>
       <c r="C43">
-        <v>0.102754530799938</v>
-      </c>
-      <c r="D43">
-        <v>0.108716625199667</v>
-      </c>
-      <c r="E43">
-        <v>0.29106894190044802</v>
+        <v>0.58325360699891404</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.63989551490067198</v>
+      </c>
+      <c r="E43" s="2">
+        <v>1.6494386505990399</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B44">
-        <v>0.20574450750009399</v>
+        <v>1.0708404860999501</v>
       </c>
       <c r="C44">
-        <v>0.108961528999861</v>
-      </c>
-      <c r="D44">
-        <v>0.119693600399477</v>
-      </c>
-      <c r="E44">
-        <v>0.30836752880004498</v>
+        <v>0.570288277900726</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0.63413740099877003</v>
+      </c>
+      <c r="E44" s="2">
+        <v>1.60557891699954</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B45">
-        <v>0.21662674379986099</v>
+        <v>1.1312382536001599</v>
       </c>
       <c r="C45">
-        <v>0.11411625899982</v>
-      </c>
-      <c r="D45">
-        <v>0.12320591430052399</v>
-      </c>
-      <c r="E45">
-        <v>0.32412643869993102</v>
+        <v>0.59794499590007</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0.66738935729954396</v>
+      </c>
+      <c r="E45" s="2">
+        <v>1.69877954600069</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B46">
-        <v>0.226218249299563</v>
+        <v>1.19357254129918</v>
       </c>
       <c r="C46">
-        <v>0.11932788869999</v>
-      </c>
-      <c r="D46">
-        <v>0.13026815089979199</v>
-      </c>
-      <c r="E46">
-        <v>0.33960566820023802</v>
+        <v>0.63024663750038601</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0.67292278480144796</v>
+      </c>
+      <c r="E46" s="2">
+        <v>1.7887417322002801</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B47">
-        <v>0.239715664400137</v>
+        <v>1.2437852959001201</v>
       </c>
       <c r="C47">
-        <v>0.125176039800135</v>
-      </c>
-      <c r="D47">
-        <v>0.13732159060018601</v>
-      </c>
-      <c r="E47">
-        <v>0.357682228499834</v>
+        <v>0.65248028640089595</v>
+      </c>
+      <c r="D47" s="2">
+        <v>0.73082350660024498</v>
+      </c>
+      <c r="E47" s="2">
+        <v>1.8637891257989301</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B48">
-        <v>0.251967093700113</v>
+        <v>1.2551267647990201</v>
       </c>
       <c r="C48">
-        <v>0.132482420799897</v>
-      </c>
-      <c r="D48">
-        <v>0.145840098199914</v>
-      </c>
-      <c r="E48">
-        <v>0.37381655209974202</v>
+        <v>0.66539579050004205</v>
+      </c>
+      <c r="D48" s="2">
+        <v>0.74921325810137196</v>
+      </c>
+      <c r="E48" s="2">
+        <v>1.8838353899993301</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B49">
-        <v>0.26526229680039198</v>
+        <v>1.2544404054002301</v>
       </c>
       <c r="C49">
-        <v>0.139515464800024</v>
-      </c>
-      <c r="D49">
-        <v>0.14627348049962099</v>
-      </c>
-      <c r="E49">
-        <v>0.39814964640008799</v>
+        <v>0.66307766690151704</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0.72098998729979902</v>
+      </c>
+      <c r="E49" s="2">
+        <v>1.8848292785993099</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="B50">
-        <v>0.28300531269996998</v>
+        <v>1.3287716202988999</v>
       </c>
       <c r="C50">
-        <v>0.147919749400171</v>
-      </c>
-      <c r="D50">
-        <v>0.16064395250013999</v>
-      </c>
-      <c r="E50">
-        <v>0.42393697019997401</v>
+        <v>0.69983272869940205</v>
+      </c>
+      <c r="D50" s="2">
+        <v>0.75770071889928603</v>
+      </c>
+      <c r="E50" s="2">
+        <v>1.9883503903994999</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B51">
-        <v>0.29699453159973899</v>
+        <v>1.41724539430069</v>
       </c>
       <c r="C51">
-        <v>0.15517947990028899</v>
-      </c>
-      <c r="D51">
-        <v>0.16888037839980799</v>
-      </c>
-      <c r="E51">
-        <v>0.44301330420002999</v>
+        <v>0.74058934510066998</v>
+      </c>
+      <c r="D51" s="2">
+        <v>0.79036957649950601</v>
+      </c>
+      <c r="E51" s="2">
+        <v>2.1270539095992702</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B52">
-        <v>0.30998000739982601</v>
+        <v>1.47993955420024</v>
       </c>
       <c r="C52">
-        <v>0.16301383559948501</v>
-      </c>
-      <c r="D52">
-        <v>0.18076914419998499</v>
-      </c>
-      <c r="E52">
-        <v>0.46559848839951801</v>
+        <v>0.77654517450136995</v>
+      </c>
+      <c r="D52" s="2">
+        <v>0.84508180389912002</v>
+      </c>
+      <c r="E52" s="2">
+        <v>2.2228912594997299</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="B53">
-        <v>0.32555256889991102</v>
+        <v>1.55903212329994</v>
       </c>
       <c r="C53">
-        <v>0.16910860999960201</v>
-      </c>
-      <c r="D53">
-        <v>0.18426371760015101</v>
-      </c>
-      <c r="E53">
-        <v>0.48670419349982602</v>
+        <v>0.81644885379937404</v>
+      </c>
+      <c r="D53" s="2">
+        <v>0.89774279399825896</v>
+      </c>
+      <c r="E53" s="2">
+        <v>2.3335044592000398</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B54">
-        <v>0.34068182669980102</v>
+        <v>1.4608146350003099</v>
       </c>
       <c r="C54">
-        <v>0.17788022569984599</v>
-      </c>
-      <c r="D54">
-        <v>0.19924401890020799</v>
-      </c>
-      <c r="E54">
-        <v>0.50938795449983398</v>
+        <v>0.76028743970018697</v>
+      </c>
+      <c r="D54" s="2">
+        <v>0.82598361469936199</v>
+      </c>
+      <c r="E54" s="2">
+        <v>2.18920955330031</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B55">
-        <v>0.35477002869902202</v>
+        <v>1.53480453409847</v>
       </c>
       <c r="C55">
-        <v>0.18526714669987901</v>
-      </c>
-      <c r="D55">
-        <v>0.199489297400396</v>
-      </c>
-      <c r="E55">
-        <v>0.534613853999508</v>
+        <v>0.796910255799957</v>
+      </c>
+      <c r="D55" s="2">
+        <v>0.84817088739910096</v>
+      </c>
+      <c r="E55" s="2">
+        <v>2.2941260346002301</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B56">
-        <v>0.37589289489951599</v>
+        <v>1.60109474610089</v>
       </c>
       <c r="C56">
-        <v>0.19429067160053801</v>
-      </c>
-      <c r="D56">
-        <v>0.218823468499795</v>
-      </c>
-      <c r="E56">
-        <v>0.55813183870013705</v>
+        <v>0.832725139601461</v>
+      </c>
+      <c r="D56" s="2">
+        <v>0.903075633001026</v>
+      </c>
+      <c r="E56" s="2">
+        <v>2.40254106720058</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B57">
-        <v>0.38700887849954502</v>
+        <v>1.6807869504003901</v>
       </c>
       <c r="C57">
-        <v>0.200878551500318</v>
-      </c>
-      <c r="D57">
-        <v>0.21788514599938899</v>
-      </c>
-      <c r="E57">
-        <v>0.57925065719919</v>
+        <v>0.87121704090040997</v>
+      </c>
+      <c r="D57" s="2">
+        <v>0.95256263920036799</v>
+      </c>
+      <c r="E57" s="2">
+        <v>2.5177176356994</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58">
+        <v>290</v>
+      </c>
+      <c r="B58">
+        <v>1.7401538370002501</v>
+      </c>
+      <c r="C58">
+        <v>0.90129282159905399</v>
+      </c>
+      <c r="D58" s="2">
+        <v>0.96567381440126998</v>
+      </c>
+      <c r="E58" s="2">
+        <v>2.60661137690149</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59">
         <v>295</v>
       </c>
-      <c r="B58">
-        <v>0.40694332049988502</v>
-      </c>
-      <c r="C58">
-        <v>0.21276150410012601</v>
-      </c>
-      <c r="D58">
-        <v>0.22706223179993601</v>
-      </c>
-      <c r="E58">
-        <v>0.61241461520057705</v>
+      <c r="B59">
+        <v>1.8368330850007599</v>
+      </c>
+      <c r="C59">
+        <v>0.96001291189877502</v>
+      </c>
+      <c r="D59" s="2">
+        <v>1.0172308631003</v>
+      </c>
+      <c r="E59" s="2">
+        <v>2.7560732964999199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
up RSA chiffrement time , total
</commit_message>
<xml_diff>
--- a/Mesures/Mesures.xlsx
+++ b/Mesures/Mesures.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14540" tabRatio="500" firstSheet="9" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14540" tabRatio="500" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Attaque Brutale" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="Miller Rabin proba" sheetId="11" r:id="rId11"/>
     <sheet name="test puiss mod" sheetId="12" r:id="rId12"/>
     <sheet name="RSA Génération" sheetId="13" r:id="rId13"/>
-    <sheet name="Chiffrement RSA" sheetId="18" r:id="rId14"/>
+    <sheet name="Feuil1" sheetId="21" r:id="rId14"/>
     <sheet name="Chiffrement EG DES" sheetId="15" r:id="rId15"/>
     <sheet name="Th des nombres premiers" sheetId="16" r:id="rId16"/>
     <sheet name="EG DES fonction de p" sheetId="20" r:id="rId17"/>
@@ -42,7 +42,7 @@
     <definedName name="Chiffrement_ElGamal_DES" localSheetId="14">'Chiffrement EG DES'!$A$1:$E$220</definedName>
     <definedName name="Chiffrement_ElGamal_fonction_de_p" localSheetId="17">'EG fonction de p'!$A$2:$E$59</definedName>
     <definedName name="Chiffrement_ElGamal_n_200" localSheetId="6">'Chiffrement El gamal'!$A$1:$E$331</definedName>
-    <definedName name="Chiffrement_RSA" localSheetId="13">'Chiffrement RSA'!$A$2:$E$165</definedName>
+    <definedName name="Chiffrement_RSA" localSheetId="13">Feuil1!$A$2:$E$232</definedName>
     <definedName name="Générateur_moy_100" localSheetId="7">'Générateur k illimité'!$A$1:$G$71</definedName>
     <definedName name="Génerateur_moy10_k_500" localSheetId="8">'Générateur 500'!$A$2:$D$58</definedName>
     <definedName name="MillerRabin_génération_moy_100" localSheetId="9">'Miller Rabin gen'!$A$1:$D$262</definedName>
@@ -151,7 +151,7 @@
     </textPr>
   </connection>
   <connection id="10" name="-Chiffrement_RSA" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="/Users/Ludo/Documents/GitHub/tipe/Mesures/-Chiffrement_RSA.txt" thousands=" " semicolon="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/Ludo/Documents/GitHub/tipe/Mesures/-Chiffrement_RSA.txt" thousands=" " semicolon="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -229,7 +229,7 @@
     </textPr>
   </connection>
   <connection id="18" name="Chiffrement EG DES var p" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/Ludo/Documents/GitHub/tipe/Mesures/Chiffrement EG DES var p.txt" thousands=" " tab="0" semicolon="1">
+    <textPr fileType="mac" sourceFile="/Users/Ludo/Documents/GitHub/tipe/Mesures/Chiffrement EG DES var p.txt" thousands=" " tab="0" semicolon="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -3496,11 +3496,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1731002896"/>
-        <c:axId val="-1731000848"/>
+        <c:axId val="-1147561648"/>
+        <c:axId val="-1142383280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1731002896"/>
+        <c:axId val="-1147561648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3557,12 +3557,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1731000848"/>
+        <c:crossAx val="-1142383280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1731000848"/>
+        <c:axId val="-1142383280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3619,7 +3619,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1731002896"/>
+        <c:crossAx val="-1147561648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5145,11 +5145,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1730946576"/>
-        <c:axId val="-1730944096"/>
+        <c:axId val="-1118654944"/>
+        <c:axId val="-1118652896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1730946576"/>
+        <c:axId val="-1118654944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5206,12 +5206,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1730944096"/>
+        <c:crossAx val="-1118652896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1730944096"/>
+        <c:axId val="-1118652896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5268,7 +5268,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1730946576"/>
+        <c:crossAx val="-1118654944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6591,11 +6591,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1730930800"/>
-        <c:axId val="-1730928320"/>
+        <c:axId val="-1122076944"/>
+        <c:axId val="-1122074880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1730930800"/>
+        <c:axId val="-1122076944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6652,12 +6652,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1730928320"/>
+        <c:crossAx val="-1122074880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1730928320"/>
+        <c:axId val="-1122074880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6714,7 +6714,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1730930800"/>
+        <c:crossAx val="-1122076944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8451,11 +8451,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1770036704"/>
-        <c:axId val="-1770034912"/>
+        <c:axId val="-1142257280"/>
+        <c:axId val="-1142929792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1770036704"/>
+        <c:axId val="-1142257280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8512,12 +8512,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1770034912"/>
+        <c:crossAx val="-1142929792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1770034912"/>
+        <c:axId val="-1142929792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8574,7 +8574,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1770036704"/>
+        <c:crossAx val="-1142257280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11736,11 +11736,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1773382880"/>
-        <c:axId val="-1773380832"/>
+        <c:axId val="-1122015536"/>
+        <c:axId val="-1122013056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1773382880"/>
+        <c:axId val="-1122015536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11797,12 +11797,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1773380832"/>
+        <c:crossAx val="-1122013056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1773380832"/>
+        <c:axId val="-1122013056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11859,7 +11859,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1773382880"/>
+        <c:crossAx val="-1122015536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -23510,15 +23510,15 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E165"/>
+  <dimension ref="A1:E232"/>
   <sheetViews>
-    <sheetView topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="L153" sqref="L153"/>
+    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
+      <selection activeCell="J218" sqref="J218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" customWidth="1"/>
     <col min="2" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
@@ -25939,392 +25939,1531 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143">
-        <v>1496</v>
+        <v>1420</v>
       </c>
       <c r="B143">
-        <v>2.3111542399994498</v>
+        <v>2.0720960937003801</v>
       </c>
       <c r="C143">
-        <v>2.3087513166989</v>
+        <v>2.0691748312092302</v>
       </c>
       <c r="D143" s="2">
-        <v>2.3078786508980502</v>
+        <v>2.0692027391996799</v>
       </c>
       <c r="E143" s="2">
-        <v>2.3142482793002199</v>
+        <v>2.07372366540657</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144">
-        <v>1579</v>
+        <v>1430</v>
       </c>
       <c r="B144">
-        <v>2.3117302255002801</v>
+        <v>2.0705924523979702</v>
       </c>
       <c r="C144">
-        <v>2.30820002760119</v>
+        <v>2.0680906570050799</v>
       </c>
       <c r="D144" s="2">
-        <v>2.3088033395000802</v>
+        <v>2.0679042965901302</v>
       </c>
       <c r="E144" s="2">
-        <v>2.3128195776003801</v>
+        <v>2.0724105174027501</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145">
-        <v>1662</v>
+        <v>1440</v>
       </c>
       <c r="B145">
-        <v>2.54227149650105</v>
+        <v>2.0705879480912701</v>
       </c>
       <c r="C145">
-        <v>2.5392136873990201</v>
+        <v>2.0678238468972201</v>
       </c>
       <c r="D145" s="2">
-        <v>2.5397528821984401</v>
+        <v>2.0679077453009</v>
       </c>
       <c r="E145" s="2">
-        <v>2.5442274139004399</v>
+        <v>2.0723383640957702</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146">
-        <v>1745</v>
+        <v>1450</v>
       </c>
       <c r="B146">
-        <v>2.5428949605011399</v>
+        <v>2.0706600775010799</v>
       </c>
       <c r="C146">
-        <v>2.53902974829579</v>
+        <v>2.0678923950079402</v>
       </c>
       <c r="D146" s="2">
-        <v>2.5400896978004299</v>
+        <v>2.0679553867943401</v>
       </c>
       <c r="E146" s="2">
-        <v>2.5443249798015999</v>
+        <v>2.0724031170960999</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147">
-        <v>1828</v>
+        <v>1460</v>
       </c>
       <c r="B147">
-        <v>2.7741687695033699</v>
+        <v>2.07057874070451</v>
       </c>
       <c r="C147">
-        <v>2.7699574161993898</v>
+        <v>2.0679062676033899</v>
       </c>
       <c r="D147" s="2">
-        <v>2.7708509844003801</v>
+        <v>2.0678635074989802</v>
       </c>
       <c r="E147" s="2">
-        <v>2.7758213149019801</v>
+        <v>2.07230520669399</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148">
-        <v>1911</v>
+        <v>1470</v>
       </c>
       <c r="B148">
-        <v>2.77523935579993</v>
+        <v>2.0708216592058299</v>
       </c>
       <c r="C148">
-        <v>2.7703980756989002</v>
+        <v>2.0679155947043899</v>
       </c>
       <c r="D148" s="2">
-        <v>2.77003198079837</v>
+        <v>2.06785510921181</v>
       </c>
       <c r="E148" s="2">
-        <v>2.77650629879972</v>
+        <v>2.0723495278012698</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149">
-        <v>1994</v>
+        <v>1480</v>
       </c>
       <c r="B149">
-        <v>3.0064893082006101</v>
+        <v>2.0707800955104099</v>
       </c>
       <c r="C149">
-        <v>3.0019949998019002</v>
+        <v>2.06799967960105</v>
       </c>
       <c r="D149" s="2">
-        <v>3.0010721826023601</v>
+        <v>2.0680231159960298</v>
       </c>
       <c r="E149" s="2">
-        <v>3.0074823880975599</v>
+        <v>2.07243159350327</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150">
-        <v>2077</v>
+        <v>1490</v>
       </c>
       <c r="B150">
-        <v>3.0047839199989501</v>
+        <v>2.07069566329446</v>
       </c>
       <c r="C150">
-        <v>3.0005700640020199</v>
+        <v>2.0678587999020199</v>
       </c>
       <c r="D150" s="2">
-        <v>3.00135763599901</v>
+        <v>2.0679111574048799</v>
       </c>
       <c r="E150" s="2">
-        <v>3.0072964612987501</v>
+        <v>2.07232910840102</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151">
-        <v>2160</v>
+        <v>1500</v>
       </c>
       <c r="B151">
-        <v>3.2354625024003298</v>
+        <v>2.30070011359784</v>
       </c>
       <c r="C151">
-        <v>3.2312648426006398</v>
+        <v>2.29770002718432</v>
       </c>
       <c r="D151" s="2">
-        <v>3.2317017569992399</v>
+        <v>2.2978121812033301</v>
       </c>
       <c r="E151" s="2">
-        <v>3.23821297069916</v>
+        <v>2.3027222027012599</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152">
-        <v>2243</v>
+        <v>1510</v>
       </c>
       <c r="B152">
-        <v>3.22337480519854</v>
+        <v>2.3005539374018502</v>
       </c>
       <c r="C152">
-        <v>3.2188382781001499</v>
+        <v>2.29789095159212</v>
       </c>
       <c r="D152" s="2">
-        <v>3.2185373202999399</v>
+        <v>2.29764857830305</v>
       </c>
       <c r="E152" s="2">
-        <v>3.2266523780042902</v>
+        <v>2.3026272077957399</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153">
-        <v>2326</v>
+        <v>1520</v>
       </c>
       <c r="B153">
-        <v>3.4530660588028601</v>
+        <v>2.3004676251002798</v>
       </c>
       <c r="C153">
-        <v>3.4469978186021701</v>
+        <v>2.2975544584027299</v>
       </c>
       <c r="D153" s="2">
-        <v>3.4468672844988699</v>
+        <v>2.2975991655926902</v>
       </c>
       <c r="E153" s="2">
-        <v>3.4548454540021298</v>
+        <v>2.30257546729844</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154">
-        <v>2409</v>
+        <v>1530</v>
       </c>
       <c r="B154">
-        <v>3.45246772610116</v>
+        <v>2.3005931348030502</v>
       </c>
       <c r="C154">
-        <v>3.4471679462021698</v>
+        <v>2.2976296178996498</v>
       </c>
       <c r="D154" s="2">
-        <v>3.4486230679009102</v>
+        <v>2.2976586021861198</v>
       </c>
       <c r="E154" s="2">
-        <v>3.4544709747977298</v>
+        <v>2.30268943030678</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155">
-        <v>2492</v>
+        <v>1540</v>
       </c>
       <c r="B155">
-        <v>3.68389598089815</v>
+        <v>2.3005707608972399</v>
       </c>
       <c r="C155">
-        <v>3.6775013342004899</v>
+        <v>2.2978951948985902</v>
       </c>
       <c r="D155" s="2">
-        <v>3.6784485956992201</v>
+        <v>2.29769265469367</v>
       </c>
       <c r="E155" s="2">
-        <v>3.6863269559984402</v>
+        <v>2.3026077083020899</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156">
-        <v>2575</v>
+        <v>1550</v>
       </c>
       <c r="B156">
-        <v>3.6827995692001401</v>
+        <v>2.3005917536982401</v>
       </c>
       <c r="C156">
-        <v>3.6775139375986301</v>
+        <v>2.2976312475002398</v>
       </c>
       <c r="D156" s="2">
-        <v>3.6774336517009898</v>
+        <v>2.2976794495989399</v>
       </c>
       <c r="E156" s="2">
-        <v>3.68622713070144</v>
+        <v>2.3026275085052399</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157">
-        <v>2658</v>
+        <v>1560</v>
       </c>
       <c r="B157">
-        <v>3.9125397755018598</v>
+        <v>2.3006975166907</v>
       </c>
       <c r="C157">
-        <v>3.9069434099015701</v>
+        <v>2.2976510313033902</v>
       </c>
       <c r="D157" s="2">
-        <v>3.9071265521011802</v>
+        <v>2.29772268109663</v>
       </c>
       <c r="E157" s="2">
-        <v>3.9152474940019601</v>
+        <v>2.30259999020199</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158">
-        <v>2741</v>
+        <v>1570</v>
       </c>
       <c r="B158">
-        <v>3.9134088366976298</v>
+        <v>2.3006617117949602</v>
       </c>
       <c r="C158">
-        <v>3.9071483164032501</v>
+        <v>2.29769101130805</v>
       </c>
       <c r="D158" s="2">
-        <v>3.9076248787019701</v>
+        <v>2.2977368232983202</v>
       </c>
       <c r="E158" s="2">
-        <v>3.9154213372996298</v>
+        <v>2.30265790840203</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159">
-        <v>2824</v>
+        <v>1580</v>
       </c>
       <c r="B159">
-        <v>4.14514273610075</v>
+        <v>2.3007212318989301</v>
       </c>
       <c r="C159">
-        <v>4.13869946940176</v>
+        <v>2.29767015700053</v>
       </c>
       <c r="D159" s="2">
-        <v>4.1380854752973297</v>
+        <v>2.2977122408017698</v>
       </c>
       <c r="E159" s="2">
-        <v>4.1484387924985597</v>
+        <v>2.3026336165072201</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160">
-        <v>2907</v>
+        <v>1590</v>
       </c>
       <c r="B160">
-        <v>4.16121216540341</v>
+        <v>2.30063289379759</v>
       </c>
       <c r="C160">
-        <v>4.1553411544995402</v>
+        <v>2.29761378159164</v>
       </c>
       <c r="D160" s="2">
-        <v>4.1548015606029303</v>
+        <v>2.2976293383879201</v>
       </c>
       <c r="E160" s="2">
-        <v>4.1654067057992501</v>
+        <v>2.30254187560785</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161">
-        <v>2990</v>
+        <v>1600</v>
       </c>
       <c r="B161">
-        <v>4.3926759652978902</v>
+        <v>2.3008301772046198</v>
       </c>
       <c r="C161">
-        <v>4.3864021097011499</v>
+        <v>2.29769532960053</v>
       </c>
       <c r="D161" s="2">
-        <v>4.3859517776989296</v>
+        <v>2.2977201544941601</v>
       </c>
       <c r="E161" s="2">
-        <v>4.3949133500027502</v>
+        <v>2.3026574744944801</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162">
-        <v>3073</v>
+        <v>1610</v>
       </c>
       <c r="B162">
-        <v>4.3934037495062501</v>
+        <v>2.3007572182017602</v>
       </c>
       <c r="C162">
-        <v>4.3853470613022996</v>
+        <v>2.2976283469993999</v>
       </c>
       <c r="D162" s="2">
-        <v>4.3859115923023602</v>
+        <v>2.2976318066022898</v>
       </c>
       <c r="E162" s="2">
-        <v>4.3953194876012196</v>
+        <v>2.3026045935024699</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163">
-        <v>3156</v>
+        <v>1620</v>
       </c>
       <c r="B163">
-        <v>4.6253574120979399</v>
+        <v>2.3008418676050399</v>
       </c>
       <c r="C163">
-        <v>4.6190958194034399</v>
+        <v>2.2976865824937698</v>
       </c>
       <c r="D163" s="2">
-        <v>4.61688279299924</v>
+        <v>2.2977102707038202</v>
       </c>
       <c r="E163" s="2">
-        <v>4.6287809478970301</v>
+        <v>2.3026691920968001</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164">
-        <v>3239</v>
+        <v>1630</v>
       </c>
       <c r="B164">
-        <v>4.6242938347939297</v>
+        <v>2.3008185796963501</v>
       </c>
       <c r="C164">
-        <v>4.6157836322919996</v>
+        <v>2.2976270771017799</v>
       </c>
       <c r="D164" s="2">
-        <v>4.6167181064934901</v>
+        <v>2.2978595245920501</v>
       </c>
       <c r="E164" s="2">
-        <v>4.6258708813016698</v>
+        <v>2.3025560449037501</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165">
+        <v>1640</v>
+      </c>
+      <c r="B165">
+        <v>2.3008330344891799</v>
+      </c>
+      <c r="C165">
+        <v>2.2975784190057298</v>
+      </c>
+      <c r="D165" s="2">
+        <v>2.2980220575016501</v>
+      </c>
+      <c r="E165" s="2">
+        <v>2.3025095215023601</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>1650</v>
+      </c>
+      <c r="B166">
+        <v>2.3008670716037098</v>
+      </c>
+      <c r="C166">
+        <v>2.2976675818063002</v>
+      </c>
+      <c r="D166" s="2">
+        <v>2.2976647921954201</v>
+      </c>
+      <c r="E166" s="2">
+        <v>2.3026430903104398</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>1660</v>
+      </c>
+      <c r="B167">
+        <v>2.5305272867059099</v>
+      </c>
+      <c r="C167">
+        <v>2.52728187599859</v>
+      </c>
+      <c r="D167" s="2">
+        <v>2.5273056788952002</v>
+      </c>
+      <c r="E167" s="2">
+        <v>2.53276405109645</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>1670</v>
+      </c>
+      <c r="B168">
+        <v>2.5304981701003202</v>
+      </c>
+      <c r="C168">
+        <v>2.5271821300964801</v>
+      </c>
+      <c r="D168" s="2">
+        <v>2.5272404727031201</v>
+      </c>
+      <c r="E168" s="2">
+        <v>2.5326604865054798</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>1680</v>
+      </c>
+      <c r="B169">
+        <v>2.53066443070129</v>
+      </c>
+      <c r="C169">
+        <v>2.5272612416170799</v>
+      </c>
+      <c r="D169" s="2">
+        <v>2.5273032679018699</v>
+      </c>
+      <c r="E169" s="2">
+        <v>2.53279350849188</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>1690</v>
+      </c>
+      <c r="B170">
+        <v>2.53068451770377</v>
+      </c>
+      <c r="C170">
+        <v>2.5273120830912301</v>
+      </c>
+      <c r="D170" s="2">
+        <v>2.5273188083054201</v>
+      </c>
+      <c r="E170" s="2">
+        <v>2.53278665270336</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>1700</v>
+      </c>
+      <c r="B171">
+        <v>2.53071243769518</v>
+      </c>
+      <c r="C171">
+        <v>2.5275462313016699</v>
+      </c>
+      <c r="D171" s="2">
+        <v>2.5273805446049602</v>
+      </c>
+      <c r="E171" s="2">
+        <v>2.53278532389667</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>1710</v>
+      </c>
+      <c r="B172">
+        <v>2.5309537319946598</v>
+      </c>
+      <c r="C172">
+        <v>2.5273667005079901</v>
+      </c>
+      <c r="D172" s="2">
+        <v>2.52733520139736</v>
+      </c>
+      <c r="E172" s="2">
+        <v>2.5330591130987101</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>1720</v>
+      </c>
+      <c r="B173">
+        <v>2.53068194241059</v>
+      </c>
+      <c r="C173">
+        <v>2.5272968736025998</v>
+      </c>
+      <c r="D173" s="2">
+        <v>2.5273239771006</v>
+      </c>
+      <c r="E173" s="2">
+        <v>2.5327500929954101</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>1730</v>
+      </c>
+      <c r="B174">
+        <v>2.5307543062997802</v>
+      </c>
+      <c r="C174">
+        <v>2.5272884985897601</v>
+      </c>
+      <c r="D174" s="2">
+        <v>2.52729106070182</v>
+      </c>
+      <c r="E174" s="2">
+        <v>2.53279036850435</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>1740</v>
+      </c>
+      <c r="B175">
+        <v>2.5308963880059299</v>
+      </c>
+      <c r="C175">
+        <v>2.5274574710012501</v>
+      </c>
+      <c r="D175" s="2">
+        <v>2.5274936164947501</v>
+      </c>
+      <c r="E175" s="2">
+        <v>2.5329108514051701</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>1750</v>
+      </c>
+      <c r="B176">
+        <v>2.5311440539095198</v>
+      </c>
+      <c r="C176">
+        <v>2.5273707643980701</v>
+      </c>
+      <c r="D176" s="2">
+        <v>2.52738549440837</v>
+      </c>
+      <c r="E176" s="2">
+        <v>2.5328881453053298</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>1760</v>
+      </c>
+      <c r="B177">
+        <v>2.53082344390713</v>
+      </c>
+      <c r="C177">
+        <v>2.52734439809573</v>
+      </c>
+      <c r="D177" s="2">
+        <v>2.5275459726937699</v>
+      </c>
+      <c r="E177" s="2">
+        <v>2.5327317103001401</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>1770</v>
+      </c>
+      <c r="B178">
+        <v>2.5307926060006101</v>
+      </c>
+      <c r="C178">
+        <v>2.5273235902000999</v>
+      </c>
+      <c r="D178" s="2">
+        <v>2.5272206981971901</v>
+      </c>
+      <c r="E178" s="2">
+        <v>2.5327349854109298</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>1780</v>
+      </c>
+      <c r="B179">
+        <v>2.5308286005049001</v>
+      </c>
+      <c r="C179">
+        <v>2.5272390729063701</v>
+      </c>
+      <c r="D179" s="2">
+        <v>2.5273326164111398</v>
+      </c>
+      <c r="E179" s="2">
+        <v>2.53277611660305</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>1790</v>
+      </c>
+      <c r="B180">
+        <v>2.5309526209020898</v>
+      </c>
+      <c r="C180">
+        <v>2.5273055284997099</v>
+      </c>
+      <c r="D180" s="2">
+        <v>2.5273402904960598</v>
+      </c>
+      <c r="E180" s="2">
+        <v>2.5329879653916501</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>1800</v>
+      </c>
+      <c r="B181">
+        <v>2.5310159043015998</v>
+      </c>
+      <c r="C181">
+        <v>2.52742368399631</v>
+      </c>
+      <c r="D181" s="2">
+        <v>2.5273960866921699</v>
+      </c>
+      <c r="E181" s="2">
+        <v>2.5329347132996101</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <v>1810</v>
+      </c>
+      <c r="B182">
+        <v>2.5310784370056298</v>
+      </c>
+      <c r="C182">
+        <v>2.52741491539782</v>
+      </c>
+      <c r="D182" s="2">
+        <v>2.52742724980344</v>
+      </c>
+      <c r="E182" s="2">
+        <v>2.5328647253074399</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>1820</v>
+      </c>
+      <c r="B183">
+        <v>2.5309292604957498</v>
+      </c>
+      <c r="C183">
+        <v>2.52743795840215</v>
+      </c>
+      <c r="D183" s="2">
+        <v>2.5272843404003602</v>
+      </c>
+      <c r="E183" s="2">
+        <v>2.5327121799040402</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <v>1830</v>
+      </c>
+      <c r="B184">
+        <v>2.7608687895975801</v>
+      </c>
+      <c r="C184">
+        <v>2.75715441230422</v>
+      </c>
+      <c r="D184" s="2">
+        <v>2.7571708193980098</v>
+      </c>
+      <c r="E184" s="2">
+        <v>2.7630478260922202</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A185">
+        <v>1840</v>
+      </c>
+      <c r="B185">
+        <v>2.7608193680964099</v>
+      </c>
+      <c r="C185">
+        <v>2.7570774131891</v>
+      </c>
+      <c r="D185" s="2">
+        <v>2.75708148060657</v>
+      </c>
+      <c r="E185" s="2">
+        <v>2.76296912371035</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A186">
+        <v>1850</v>
+      </c>
+      <c r="B186">
+        <v>2.7611621199874201</v>
+      </c>
+      <c r="C186">
+        <v>2.7571974591148298</v>
+      </c>
+      <c r="D186" s="2">
+        <v>2.7571940436930098</v>
+      </c>
+      <c r="E186" s="2">
+        <v>2.7631355020930601</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A187">
+        <v>1860</v>
+      </c>
+      <c r="B187">
+        <v>2.7608670094079502</v>
+      </c>
+      <c r="C187">
+        <v>2.75702316570968</v>
+      </c>
+      <c r="D187" s="2">
+        <v>2.75701197850867</v>
+      </c>
+      <c r="E187" s="2">
+        <v>2.76300176469812</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A188">
+        <v>1870</v>
+      </c>
+      <c r="B188">
+        <v>2.76138985950237</v>
+      </c>
+      <c r="C188">
+        <v>2.7574441263030098</v>
+      </c>
+      <c r="D188" s="2">
+        <v>2.7571849455940498</v>
+      </c>
+      <c r="E188" s="2">
+        <v>2.7630546594038599</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A189">
+        <v>1880</v>
+      </c>
+      <c r="B189">
+        <v>2.7608408778964</v>
+      </c>
+      <c r="C189">
+        <v>2.7570014780023402</v>
+      </c>
+      <c r="D189" s="2">
+        <v>2.7570023840060398</v>
+      </c>
+      <c r="E189" s="2">
+        <v>2.7629409994013199</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A190">
+        <v>1890</v>
+      </c>
+      <c r="B190">
+        <v>2.7608779274087198</v>
+      </c>
+      <c r="C190">
+        <v>2.75697243930771</v>
+      </c>
+      <c r="D190" s="2">
+        <v>2.75699492249987</v>
+      </c>
+      <c r="E190" s="2">
+        <v>2.76294830340048</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A191">
+        <v>1900</v>
+      </c>
+      <c r="B191">
+        <v>2.7611057529109502</v>
+      </c>
+      <c r="C191">
+        <v>2.7571451764059001</v>
+      </c>
+      <c r="D191" s="2">
+        <v>2.7571732121024901</v>
+      </c>
+      <c r="E191" s="2">
+        <v>2.7630890867993001</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A192">
+        <v>1910</v>
+      </c>
+      <c r="B192">
+        <v>2.76123205699695</v>
+      </c>
+      <c r="C192">
+        <v>2.7572152980108502</v>
+      </c>
+      <c r="D192" s="2">
+        <v>2.7572263089867102</v>
+      </c>
+      <c r="E192" s="2">
+        <v>2.7634342884994099</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A193">
+        <v>1920</v>
+      </c>
+      <c r="B193">
+        <v>2.7610606962945798</v>
+      </c>
+      <c r="C193">
+        <v>2.7570433864035202</v>
+      </c>
+      <c r="D193" s="2">
+        <v>2.7570587661975798</v>
+      </c>
+      <c r="E193" s="2">
+        <v>2.7630237922858201</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A194">
+        <v>1930</v>
+      </c>
+      <c r="B194">
+        <v>2.76154333680606</v>
+      </c>
+      <c r="C194">
+        <v>2.7572645066000399</v>
+      </c>
+      <c r="D194" s="2">
+        <v>2.7570956582174402</v>
+      </c>
+      <c r="E194" s="2">
+        <v>2.76321785648615</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A195">
+        <v>1940</v>
+      </c>
+      <c r="B195">
+        <v>2.7620819208968799</v>
+      </c>
+      <c r="C195">
+        <v>2.7580681402061602</v>
+      </c>
+      <c r="D195" s="2">
+        <v>2.75871649960026</v>
+      </c>
+      <c r="E195" s="2">
+        <v>2.76410734370147</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A196">
+        <v>1950</v>
+      </c>
+      <c r="B196">
+        <v>2.7625557917053798</v>
+      </c>
+      <c r="C196">
+        <v>2.7585151931009002</v>
+      </c>
+      <c r="D196" s="2">
+        <v>2.7584986772024398</v>
+      </c>
+      <c r="E196" s="2">
+        <v>2.76446683601243</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A197">
+        <v>1960</v>
+      </c>
+      <c r="B197">
+        <v>2.7622497286065402</v>
+      </c>
+      <c r="C197">
+        <v>2.7579799120998301</v>
+      </c>
+      <c r="D197" s="2">
+        <v>2.7579366677993602</v>
+      </c>
+      <c r="E197" s="2">
+        <v>2.7641169813126898</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A198">
+        <v>1970</v>
+      </c>
+      <c r="B198">
+        <v>2.7619317531061802</v>
+      </c>
+      <c r="C198">
+        <v>2.7576033735007499</v>
+      </c>
+      <c r="D198" s="2">
+        <v>2.7576439408934599</v>
+      </c>
+      <c r="E198" s="2">
+        <v>2.7635942614011499</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A199">
+        <v>1980</v>
+      </c>
+      <c r="B199">
+        <v>2.7621343967984999</v>
+      </c>
+      <c r="C199">
+        <v>2.75762524890742</v>
+      </c>
+      <c r="D199" s="2">
+        <v>2.75771496130037</v>
+      </c>
+      <c r="E199" s="2">
+        <v>2.7638953733970899</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A200">
+        <v>1990</v>
+      </c>
+      <c r="B200">
+        <v>2.76212112910288</v>
+      </c>
+      <c r="C200">
+        <v>2.7580158733922802</v>
+      </c>
+      <c r="D200" s="2">
+        <v>2.75805243010254</v>
+      </c>
+      <c r="E200" s="2">
+        <v>2.7638678199043998</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A201">
+        <v>2000</v>
+      </c>
+      <c r="B201">
+        <v>2.99149814789561</v>
+      </c>
+      <c r="C201">
+        <v>2.9871884398045898</v>
+      </c>
+      <c r="D201" s="2">
+        <v>2.9871647003950699</v>
+      </c>
+      <c r="E201" s="2">
+        <v>2.9938768494961501</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A202">
+        <v>2010</v>
+      </c>
+      <c r="B202">
+        <v>2.9916805821994701</v>
+      </c>
+      <c r="C202">
+        <v>2.9875551333025201</v>
+      </c>
+      <c r="D202" s="2">
+        <v>2.98730889559083</v>
+      </c>
+      <c r="E202" s="2">
+        <v>2.9939588671913899</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A203">
+        <v>2020</v>
+      </c>
+      <c r="B203">
+        <v>2.9917597733030501</v>
+      </c>
+      <c r="C203">
+        <v>2.98752199860464</v>
+      </c>
+      <c r="D203" s="2">
+        <v>2.98757557519711</v>
+      </c>
+      <c r="E203" s="2">
+        <v>2.99389880969101</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A204">
+        <v>2030</v>
+      </c>
+      <c r="B204">
+        <v>2.99318716910784</v>
+      </c>
+      <c r="C204">
+        <v>2.9886633948044601</v>
+      </c>
+      <c r="D204" s="2">
+        <v>2.98879685250576</v>
+      </c>
+      <c r="E204" s="2">
+        <v>2.9949502029077801</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A205">
+        <v>2040</v>
+      </c>
+      <c r="B205">
+        <v>2.99214607378235</v>
+      </c>
+      <c r="C205">
+        <v>2.9875759397968</v>
+      </c>
+      <c r="D205" s="2">
+        <v>2.9877137569113899</v>
+      </c>
+      <c r="E205" s="2">
+        <v>2.9940743668979799</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A206">
+        <v>2050</v>
+      </c>
+      <c r="B206">
+        <v>2.9926699243034798</v>
+      </c>
+      <c r="C206">
+        <v>2.98808183140499</v>
+      </c>
+      <c r="D206" s="2">
+        <v>2.9880063222910298</v>
+      </c>
+      <c r="E206" s="2">
+        <v>2.9944760921120102</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A207">
+        <v>2060</v>
+      </c>
+      <c r="B207">
+        <v>2.9923351133940699</v>
+      </c>
+      <c r="C207">
+        <v>2.9877558735970502</v>
+      </c>
+      <c r="D207" s="2">
+        <v>2.9877930198082998</v>
+      </c>
+      <c r="E207" s="2">
+        <v>2.9941034748000601</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A208">
+        <v>2070</v>
+      </c>
+      <c r="B208">
+        <v>2.9923910543016898</v>
+      </c>
+      <c r="C208">
+        <v>2.98841272720892</v>
+      </c>
+      <c r="D208" s="2">
+        <v>2.9879152475084898</v>
+      </c>
+      <c r="E208" s="2">
+        <v>2.9945542739980699</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A209">
+        <v>2080</v>
+      </c>
+      <c r="B209">
+        <v>2.99232054179592</v>
+      </c>
+      <c r="C209">
+        <v>2.9877967609005198</v>
+      </c>
+      <c r="D209" s="2">
+        <v>2.9877273601887202</v>
+      </c>
+      <c r="E209" s="2">
+        <v>2.99408877420501</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A210">
+        <v>2090</v>
+      </c>
+      <c r="B210">
+        <v>2.9925553643130098</v>
+      </c>
+      <c r="C210">
+        <v>2.98837256490514</v>
+      </c>
+      <c r="D210" s="2">
+        <v>2.98836442491156</v>
+      </c>
+      <c r="E210" s="2">
+        <v>2.9949206128119799</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A211">
+        <v>2100</v>
+      </c>
+      <c r="B211">
+        <v>2.99172748579731</v>
+      </c>
+      <c r="C211">
+        <v>2.98731999228912</v>
+      </c>
+      <c r="D211" s="2">
+        <v>2.9872641336027299</v>
+      </c>
+      <c r="E211" s="2">
+        <v>2.9938582106027698</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A212">
+        <v>2110</v>
+      </c>
+      <c r="B212">
+        <v>2.9924594732976399</v>
+      </c>
+      <c r="C212">
+        <v>2.9876960176916301</v>
+      </c>
+      <c r="D212" s="2">
+        <v>2.9879041209002</v>
+      </c>
+      <c r="E212" s="2">
+        <v>2.9940195506133001</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A213">
+        <v>2120</v>
+      </c>
+      <c r="B213">
+        <v>2.9922885200037799</v>
+      </c>
+      <c r="C213">
+        <v>2.9877870161042601</v>
+      </c>
+      <c r="D213" s="2">
+        <v>2.9877076259915998</v>
+      </c>
+      <c r="E213" s="2">
+        <v>2.9942102662869701</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A214">
+        <v>2130</v>
+      </c>
+      <c r="B214">
+        <v>2.9920565453925501</v>
+      </c>
+      <c r="C214">
+        <v>2.9877459868017402</v>
+      </c>
+      <c r="D214" s="2">
+        <v>2.9873948755120998</v>
+      </c>
+      <c r="E214" s="2">
+        <v>2.9941189787234102</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A215">
+        <v>2140</v>
+      </c>
+      <c r="B215">
+        <v>2.9912141688037002</v>
+      </c>
+      <c r="C215">
+        <v>2.9868234042005399</v>
+      </c>
+      <c r="D215" s="2">
+        <v>2.9868312951060898</v>
+      </c>
+      <c r="E215" s="2">
+        <v>2.99319127950002</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A216">
+        <v>2150</v>
+      </c>
+      <c r="B216">
+        <v>2.9914225347994901</v>
+      </c>
+      <c r="C216">
+        <v>2.98696860851341</v>
+      </c>
+      <c r="D216" s="2">
+        <v>2.9868383380948198</v>
+      </c>
+      <c r="E216" s="2">
+        <v>2.9933183495959299</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A217">
+        <v>2160</v>
+      </c>
+      <c r="B217">
+        <v>3.2213564138000899</v>
+      </c>
+      <c r="C217">
+        <v>3.2168450827113699</v>
+      </c>
+      <c r="D217" s="2">
+        <v>3.2168169995013098</v>
+      </c>
+      <c r="E217" s="2">
+        <v>3.2238696464948502</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A218">
+        <v>2170</v>
+      </c>
+      <c r="B218">
+        <v>3.22148974949959</v>
+      </c>
+      <c r="C218">
+        <v>3.21700466649781</v>
+      </c>
+      <c r="D218" s="2">
+        <v>3.2170472866055202</v>
+      </c>
+      <c r="E218" s="2">
+        <v>3.22404391820309</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A219">
+        <v>2243</v>
+      </c>
+      <c r="B219">
+        <v>3.22337480519854</v>
+      </c>
+      <c r="C219">
+        <v>3.2188382781001499</v>
+      </c>
+      <c r="D219" s="2">
+        <v>3.2185373202999399</v>
+      </c>
+      <c r="E219" s="2">
+        <v>3.2266523780042902</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A220">
+        <v>2326</v>
+      </c>
+      <c r="B220">
+        <v>3.4530660588028601</v>
+      </c>
+      <c r="C220">
+        <v>3.4469978186021701</v>
+      </c>
+      <c r="D220" s="2">
+        <v>3.4468672844988699</v>
+      </c>
+      <c r="E220" s="2">
+        <v>3.4548454540021298</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A221">
+        <v>2409</v>
+      </c>
+      <c r="B221">
+        <v>3.45246772610116</v>
+      </c>
+      <c r="C221">
+        <v>3.4471679462021698</v>
+      </c>
+      <c r="D221" s="2">
+        <v>3.4486230679009102</v>
+      </c>
+      <c r="E221" s="2">
+        <v>3.4544709747977298</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A222">
+        <v>2492</v>
+      </c>
+      <c r="B222">
+        <v>3.68389598089815</v>
+      </c>
+      <c r="C222">
+        <v>3.6775013342004899</v>
+      </c>
+      <c r="D222" s="2">
+        <v>3.6784485956992201</v>
+      </c>
+      <c r="E222" s="2">
+        <v>3.6863269559984402</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A223">
+        <v>2575</v>
+      </c>
+      <c r="B223">
+        <v>3.6827995692001401</v>
+      </c>
+      <c r="C223">
+        <v>3.6775139375986301</v>
+      </c>
+      <c r="D223" s="2">
+        <v>3.6774336517009898</v>
+      </c>
+      <c r="E223" s="2">
+        <v>3.68622713070144</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A224">
+        <v>2658</v>
+      </c>
+      <c r="B224">
+        <v>3.9125397755018598</v>
+      </c>
+      <c r="C224">
+        <v>3.9069434099015701</v>
+      </c>
+      <c r="D224" s="2">
+        <v>3.9071265521011802</v>
+      </c>
+      <c r="E224" s="2">
+        <v>3.9152474940019601</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A225">
+        <v>2741</v>
+      </c>
+      <c r="B225">
+        <v>3.9134088366976298</v>
+      </c>
+      <c r="C225">
+        <v>3.9071483164032501</v>
+      </c>
+      <c r="D225" s="2">
+        <v>3.9076248787019701</v>
+      </c>
+      <c r="E225" s="2">
+        <v>3.9154213372996298</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A226">
+        <v>2824</v>
+      </c>
+      <c r="B226">
+        <v>4.14514273610075</v>
+      </c>
+      <c r="C226">
+        <v>4.13869946940176</v>
+      </c>
+      <c r="D226" s="2">
+        <v>4.1380854752973297</v>
+      </c>
+      <c r="E226" s="2">
+        <v>4.1484387924985597</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A227">
+        <v>2907</v>
+      </c>
+      <c r="B227">
+        <v>4.16121216540341</v>
+      </c>
+      <c r="C227">
+        <v>4.1553411544995402</v>
+      </c>
+      <c r="D227" s="2">
+        <v>4.1548015606029303</v>
+      </c>
+      <c r="E227" s="2">
+        <v>4.1654067057992501</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A228">
+        <v>2990</v>
+      </c>
+      <c r="B228">
+        <v>4.3926759652978902</v>
+      </c>
+      <c r="C228">
+        <v>4.3864021097011499</v>
+      </c>
+      <c r="D228" s="2">
+        <v>4.3859517776989296</v>
+      </c>
+      <c r="E228" s="2">
+        <v>4.3949133500027502</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A229">
+        <v>3073</v>
+      </c>
+      <c r="B229">
+        <v>4.3934037495062501</v>
+      </c>
+      <c r="C229">
+        <v>4.3853470613022996</v>
+      </c>
+      <c r="D229" s="2">
+        <v>4.3859115923023602</v>
+      </c>
+      <c r="E229" s="2">
+        <v>4.3953194876012196</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A230">
+        <v>3156</v>
+      </c>
+      <c r="B230">
+        <v>4.6253574120979399</v>
+      </c>
+      <c r="C230">
+        <v>4.6190958194034399</v>
+      </c>
+      <c r="D230" s="2">
+        <v>4.61688279299924</v>
+      </c>
+      <c r="E230" s="2">
+        <v>4.6287809478970301</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A231">
+        <v>3239</v>
+      </c>
+      <c r="B231">
+        <v>4.6242938347939297</v>
+      </c>
+      <c r="C231">
+        <v>4.6157836322919996</v>
+      </c>
+      <c r="D231" s="2">
+        <v>4.6167181064934901</v>
+      </c>
+      <c r="E231" s="2">
+        <v>4.6258708813016698</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A232">
         <v>3322</v>
       </c>
-      <c r="B165">
+      <c r="B232">
         <v>4.8561269555982998</v>
       </c>
-      <c r="C165">
+      <c r="C232">
         <v>4.8499624816984497</v>
       </c>
-      <c r="D165" s="2">
+      <c r="D232" s="2">
         <v>4.8485004974027097</v>
       </c>
-      <c r="E165" s="2">
+      <c r="E232" s="2">
         <v>4.8606518181935803</v>
       </c>
     </row>
@@ -26339,7 +27478,7 @@
   <dimension ref="A1:K258"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C220"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -32288,7 +33427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -32955,7 +34094,7 @@
   <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -33970,6 +35109,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>